<commit_message>
finish 3 daily entry summit to db
</commit_message>
<xml_diff>
--- a/zoe_documents/网页设计 zoe.xlsx
+++ b/zoe_documents/网页设计 zoe.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWeb\Zoe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ritchie\Documents\financial-computing-app\zoe_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="23040" windowHeight="10935"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="23040" windowHeight="10940" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="公司信息" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="客户报告" sheetId="5" r:id="rId6"/>
     <sheet name="员工报告" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2325,7 +2325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2749,12 +2749,6 @@
     <xf numFmtId="0" fontId="16" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2772,12 +2766,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2858,21 +2846,66 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2894,53 +2927,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3078,7 +3066,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8035E939-033C-4405-97D4-C15A2CD78939}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8035E939-033C-4405-97D4-C15A2CD78939}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3406,30 +3394,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="A114" sqref="A114:XFD118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="3"/>
-    <col min="2" max="2" width="28.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="2"/>
-    <col min="11" max="11" width="12.625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.75" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16.875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.875" style="2"/>
-    <col min="15" max="15" width="8.875" style="4"/>
+    <col min="1" max="1" width="8.90625" style="3"/>
+    <col min="2" max="2" width="28.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" style="2"/>
+    <col min="11" max="11" width="12.6328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.90625" style="2"/>
+    <col min="15" max="15" width="8.90625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75">
+    <row r="1" spans="1:15" ht="15.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3836,7 +3824,7 @@
       <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="B16" s="207" t="s">
+      <c r="B16" s="196" t="s">
         <v>154</v>
       </c>
       <c r="C16" s="85" t="s">
@@ -3853,7 +3841,7 @@
       <c r="J16" s="60"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="208"/>
+      <c r="B17" s="197"/>
       <c r="C17" s="84" t="s">
         <v>61</v>
       </c>
@@ -3866,7 +3854,7 @@
       <c r="J17" s="59"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="208"/>
+      <c r="B18" s="197"/>
       <c r="C18" s="84" t="s">
         <v>62</v>
       </c>
@@ -3879,7 +3867,7 @@
       <c r="J18" s="59"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="208"/>
+      <c r="B19" s="197"/>
       <c r="C19" s="84" t="s">
         <v>100</v>
       </c>
@@ -3893,7 +3881,7 @@
       <c r="K19" s="58"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="208"/>
+      <c r="B20" s="197"/>
       <c r="C20" s="84" t="s">
         <v>101</v>
       </c>
@@ -3909,7 +3897,7 @@
       <c r="K20" s="58"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="208"/>
+      <c r="B21" s="197"/>
       <c r="C21" s="77" t="s">
         <v>87</v>
       </c>
@@ -3923,7 +3911,7 @@
       <c r="K21" s="58"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="208"/>
+      <c r="B22" s="197"/>
       <c r="C22" s="77" t="s">
         <v>88</v>
       </c>
@@ -3938,7 +3926,7 @@
       <c r="J22" s="59"/>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="208"/>
+      <c r="B23" s="197"/>
       <c r="C23" s="84" t="s">
         <v>89</v>
       </c>
@@ -3952,7 +3940,7 @@
       <c r="I23" s="61"/>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="208"/>
+      <c r="B24" s="197"/>
       <c r="C24" s="77" t="s">
         <v>92</v>
       </c>
@@ -3967,7 +3955,7 @@
       <c r="I24" s="61"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="208"/>
+      <c r="B25" s="197"/>
       <c r="C25" s="84" t="s">
         <v>94</v>
       </c>
@@ -3984,7 +3972,7 @@
       <c r="K25" s="110"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="208"/>
+      <c r="B26" s="197"/>
       <c r="C26" s="84" t="s">
         <v>95</v>
       </c>
@@ -4001,7 +3989,7 @@
       <c r="K26" s="59"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="208"/>
+      <c r="B27" s="197"/>
       <c r="C27" s="77" t="s">
         <v>102</v>
       </c>
@@ -4014,7 +4002,7 @@
       <c r="I27" s="61"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="208"/>
+      <c r="B28" s="197"/>
       <c r="C28" s="77" t="s">
         <v>103</v>
       </c>
@@ -4027,7 +4015,7 @@
       <c r="I28" s="61"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="208"/>
+      <c r="B29" s="197"/>
       <c r="C29" s="84" t="s">
         <v>199</v>
       </c>
@@ -4038,7 +4026,7 @@
       <c r="I29" s="61"/>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="208"/>
+      <c r="B30" s="197"/>
       <c r="C30" s="84" t="s">
         <v>200</v>
       </c>
@@ -4049,7 +4037,7 @@
       <c r="I30" s="61"/>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="208"/>
+      <c r="B31" s="197"/>
       <c r="C31" s="84" t="s">
         <v>202</v>
       </c>
@@ -4062,7 +4050,7 @@
       <c r="I31" s="61"/>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="208"/>
+      <c r="B32" s="197"/>
       <c r="C32" s="84" t="s">
         <v>203</v>
       </c>
@@ -4073,7 +4061,7 @@
       <c r="I32" s="61"/>
     </row>
     <row r="33" spans="2:9">
-      <c r="B33" s="208"/>
+      <c r="B33" s="197"/>
       <c r="C33" s="84" t="s">
         <v>67</v>
       </c>
@@ -4084,7 +4072,7 @@
       <c r="I33" s="61"/>
     </row>
     <row r="34" spans="2:9">
-      <c r="B34" s="208"/>
+      <c r="B34" s="197"/>
       <c r="C34" s="84" t="s">
         <v>68</v>
       </c>
@@ -4094,7 +4082,7 @@
       <c r="I34" s="61"/>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="208"/>
+      <c r="B35" s="197"/>
       <c r="C35" s="84" t="s">
         <v>69</v>
       </c>
@@ -4104,7 +4092,7 @@
       <c r="I35" s="61"/>
     </row>
     <row r="36" spans="2:9" ht="15" thickBot="1">
-      <c r="B36" s="209"/>
+      <c r="B36" s="198"/>
       <c r="C36" s="90" t="s">
         <v>72</v>
       </c>
@@ -4116,7 +4104,7 @@
       <c r="I36" s="61"/>
     </row>
     <row r="37" spans="2:9">
-      <c r="B37" s="195" t="s">
+      <c r="B37" s="199" t="s">
         <v>148</v>
       </c>
       <c r="C37" s="93" t="s">
@@ -4130,7 +4118,7 @@
       <c r="I37" s="61"/>
     </row>
     <row r="38" spans="2:9">
-      <c r="B38" s="210"/>
+      <c r="B38" s="200"/>
       <c r="C38" s="77" t="s">
         <v>126</v>
       </c>
@@ -4142,7 +4130,7 @@
       <c r="I38" s="61"/>
     </row>
     <row r="39" spans="2:9" ht="15" thickBot="1">
-      <c r="B39" s="210"/>
+      <c r="B39" s="200"/>
       <c r="C39" s="77" t="s">
         <v>121</v>
       </c>
@@ -4156,7 +4144,7 @@
       <c r="I39" s="61"/>
     </row>
     <row r="40" spans="2:9">
-      <c r="B40" s="210"/>
+      <c r="B40" s="200"/>
       <c r="C40" s="77" t="s">
         <v>135</v>
       </c>
@@ -4168,7 +4156,7 @@
       <c r="I40" s="61"/>
     </row>
     <row r="41" spans="2:9" ht="15" thickBot="1">
-      <c r="B41" s="210"/>
+      <c r="B41" s="200"/>
       <c r="C41" s="77" t="s">
         <v>125</v>
       </c>
@@ -4180,7 +4168,7 @@
       <c r="I41" s="61"/>
     </row>
     <row r="42" spans="2:9">
-      <c r="B42" s="210"/>
+      <c r="B42" s="200"/>
       <c r="C42" s="77" t="s">
         <v>136</v>
       </c>
@@ -4192,7 +4180,7 @@
       <c r="I42" s="61"/>
     </row>
     <row r="43" spans="2:9">
-      <c r="B43" s="210"/>
+      <c r="B43" s="200"/>
       <c r="C43" s="77" t="s">
         <v>230</v>
       </c>
@@ -4204,7 +4192,7 @@
       <c r="I43" s="61"/>
     </row>
     <row r="44" spans="2:9">
-      <c r="B44" s="210"/>
+      <c r="B44" s="200"/>
       <c r="C44" s="77" t="s">
         <v>231</v>
       </c>
@@ -4216,7 +4204,7 @@
       <c r="I44" s="61"/>
     </row>
     <row r="45" spans="2:9">
-      <c r="B45" s="210"/>
+      <c r="B45" s="200"/>
       <c r="C45" s="77" t="s">
         <v>232</v>
       </c>
@@ -4228,7 +4216,7 @@
       <c r="I45" s="61"/>
     </row>
     <row r="46" spans="2:9">
-      <c r="B46" s="210"/>
+      <c r="B46" s="200"/>
       <c r="C46" s="77" t="s">
         <v>137</v>
       </c>
@@ -4240,7 +4228,7 @@
       <c r="I46" s="61"/>
     </row>
     <row r="47" spans="2:9">
-      <c r="B47" s="210"/>
+      <c r="B47" s="200"/>
       <c r="C47" s="77" t="s">
         <v>129</v>
       </c>
@@ -4252,7 +4240,7 @@
       <c r="I47" s="61"/>
     </row>
     <row r="48" spans="2:9">
-      <c r="B48" s="211"/>
+      <c r="B48" s="201"/>
       <c r="C48" s="77" t="s">
         <v>162</v>
       </c>
@@ -4264,7 +4252,7 @@
       <c r="I48" s="61"/>
     </row>
     <row r="49" spans="2:9" ht="15" thickBot="1">
-      <c r="B49" s="196"/>
+      <c r="B49" s="202"/>
       <c r="C49" s="95" t="s">
         <v>130</v>
       </c>
@@ -4276,7 +4264,7 @@
       <c r="I49" s="61"/>
     </row>
     <row r="50" spans="2:9">
-      <c r="B50" s="195" t="s">
+      <c r="B50" s="199" t="s">
         <v>131</v>
       </c>
       <c r="C50" s="93" t="s">
@@ -4290,7 +4278,7 @@
       <c r="I50" s="61"/>
     </row>
     <row r="51" spans="2:9" ht="15" thickBot="1">
-      <c r="B51" s="196"/>
+      <c r="B51" s="202"/>
       <c r="C51" s="95" t="s">
         <v>131</v>
       </c>
@@ -4302,7 +4290,7 @@
       <c r="I51" s="61"/>
     </row>
     <row r="52" spans="2:9">
-      <c r="B52" s="195" t="s">
+      <c r="B52" s="199" t="s">
         <v>132</v>
       </c>
       <c r="C52" s="93" t="s">
@@ -4316,7 +4304,7 @@
       <c r="I52" s="61"/>
     </row>
     <row r="53" spans="2:9" ht="15" thickBot="1">
-      <c r="B53" s="196"/>
+      <c r="B53" s="202"/>
       <c r="C53" s="95" t="s">
         <v>132</v>
       </c>
@@ -4328,7 +4316,7 @@
       <c r="I53" s="61"/>
     </row>
     <row r="54" spans="2:9">
-      <c r="B54" s="195" t="s">
+      <c r="B54" s="199" t="s">
         <v>163</v>
       </c>
       <c r="C54" s="93" t="s">
@@ -4342,7 +4330,7 @@
       <c r="I54" s="61"/>
     </row>
     <row r="55" spans="2:9" ht="15" thickBot="1">
-      <c r="B55" s="196"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="95" t="s">
         <v>165</v>
       </c>
@@ -4354,7 +4342,7 @@
       <c r="I55" s="61"/>
     </row>
     <row r="56" spans="2:9" ht="15" thickBot="1">
-      <c r="B56" s="204" t="s">
+      <c r="B56" s="203" t="s">
         <v>150</v>
       </c>
       <c r="C56" s="93" t="s">
@@ -4368,7 +4356,7 @@
       <c r="I56" s="61"/>
     </row>
     <row r="57" spans="2:9" ht="15" thickBot="1">
-      <c r="B57" s="206"/>
+      <c r="B57" s="204"/>
       <c r="C57" s="95" t="s">
         <v>147</v>
       </c>
@@ -4380,7 +4368,7 @@
       <c r="I57" s="61"/>
     </row>
     <row r="58" spans="2:9">
-      <c r="B58" s="207" t="s">
+      <c r="B58" s="196" t="s">
         <v>151</v>
       </c>
       <c r="C58" s="93" t="s">
@@ -4394,31 +4382,31 @@
       <c r="I58" s="61"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="208"/>
+      <c r="B59" s="197"/>
       <c r="C59" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="214" t="s">
+      <c r="D59" s="190" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="215"/>
+      <c r="E59" s="191"/>
       <c r="H59" s="61"/>
       <c r="I59" s="61"/>
     </row>
     <row r="60" spans="2:9" ht="15" thickBot="1">
-      <c r="B60" s="209"/>
+      <c r="B60" s="198"/>
       <c r="C60" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="216" t="s">
+      <c r="D60" s="192" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="217"/>
+      <c r="E60" s="193"/>
       <c r="H60" s="61"/>
       <c r="I60" s="61"/>
     </row>
     <row r="61" spans="2:9">
-      <c r="B61" s="204" t="s">
+      <c r="B61" s="203" t="s">
         <v>152</v>
       </c>
       <c r="C61" s="93" t="s">
@@ -4432,7 +4420,7 @@
       <c r="I61" s="61"/>
     </row>
     <row r="62" spans="2:9">
-      <c r="B62" s="205"/>
+      <c r="B62" s="215"/>
       <c r="C62" s="77" t="s">
         <v>128</v>
       </c>
@@ -4444,7 +4432,7 @@
       <c r="I62" s="61"/>
     </row>
     <row r="63" spans="2:9" ht="15" thickBot="1">
-      <c r="B63" s="206"/>
+      <c r="B63" s="204"/>
       <c r="C63" s="95" t="s">
         <v>134</v>
       </c>
@@ -4456,7 +4444,7 @@
       <c r="I63" s="61"/>
     </row>
     <row r="64" spans="2:9">
-      <c r="B64" s="207" t="s">
+      <c r="B64" s="196" t="s">
         <v>153</v>
       </c>
       <c r="C64" s="93" t="s">
@@ -4470,7 +4458,7 @@
       <c r="I64" s="61"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="B65" s="208"/>
+      <c r="B65" s="197"/>
       <c r="C65" s="77" t="s">
         <v>145</v>
       </c>
@@ -4482,7 +4470,7 @@
       <c r="I65" s="61"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="B66" s="208"/>
+      <c r="B66" s="197"/>
       <c r="C66" s="77" t="s">
         <v>142</v>
       </c>
@@ -4494,7 +4482,7 @@
       <c r="I66" s="61"/>
     </row>
     <row r="67" spans="1:10" ht="15" thickBot="1">
-      <c r="B67" s="209"/>
+      <c r="B67" s="198"/>
       <c r="C67" s="95" t="s">
         <v>144</v>
       </c>
@@ -4506,21 +4494,21 @@
       <c r="I67" s="61"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="B68" s="192" t="s">
+      <c r="B68" s="205" t="s">
         <v>157</v>
       </c>
       <c r="C68" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="218" t="s">
+      <c r="D68" s="194" t="s">
         <v>118</v>
       </c>
-      <c r="E68" s="219"/>
+      <c r="E68" s="195"/>
       <c r="H68" s="61"/>
       <c r="I68" s="61"/>
     </row>
     <row r="69" spans="1:10" ht="15" thickBot="1">
-      <c r="B69" s="193"/>
+      <c r="B69" s="206"/>
       <c r="C69" s="103" t="s">
         <v>167</v>
       </c>
@@ -4532,7 +4520,7 @@
       <c r="I69" s="61"/>
     </row>
     <row r="70" spans="1:10" ht="15" thickBot="1">
-      <c r="B70" s="194"/>
+      <c r="B70" s="207"/>
       <c r="C70" s="91" t="s">
         <v>156</v>
       </c>
@@ -4549,16 +4537,16 @@
     </row>
     <row r="72" spans="1:10" ht="15" thickBot="1">
       <c r="B72" s="59"/>
-      <c r="C72" s="212"/>
-      <c r="D72" s="212"/>
-      <c r="E72" s="212"/>
-      <c r="F72" s="212"/>
+      <c r="C72" s="188"/>
+      <c r="D72" s="188"/>
+      <c r="E72" s="188"/>
+      <c r="F72" s="188"/>
       <c r="H72" s="61"/>
       <c r="I72" s="61"/>
       <c r="J72" s="59"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="B73" s="200" t="s">
+      <c r="B73" s="211" t="s">
         <v>85</v>
       </c>
       <c r="C73" s="116" t="s">
@@ -4578,7 +4566,7 @@
       <c r="J73" s="59"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="B74" s="201"/>
+      <c r="B74" s="212"/>
       <c r="C74" s="63" t="s">
         <v>143</v>
       </c>
@@ -4596,7 +4584,7 @@
       <c r="J74" s="59"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="B75" s="201"/>
+      <c r="B75" s="212"/>
       <c r="C75" s="63" t="s">
         <v>66</v>
       </c>
@@ -4613,7 +4601,7 @@
       <c r="I75" s="61"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="B76" s="201"/>
+      <c r="B76" s="212"/>
       <c r="C76" s="62" t="s">
         <v>64</v>
       </c>
@@ -4630,7 +4618,7 @@
       <c r="I76" s="61"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="B77" s="202"/>
+      <c r="B77" s="213"/>
       <c r="C77" s="114" t="s">
         <v>204</v>
       </c>
@@ -4647,7 +4635,7 @@
       <c r="I77" s="61"/>
     </row>
     <row r="78" spans="1:10" ht="15" thickBot="1">
-      <c r="B78" s="203"/>
+      <c r="B78" s="214"/>
       <c r="C78" s="69" t="s">
         <v>68</v>
       </c>
@@ -4674,15 +4662,15 @@
         <v>46</v>
       </c>
       <c r="B80" s="59"/>
-      <c r="C80" s="212"/>
-      <c r="D80" s="212"/>
-      <c r="E80" s="212"/>
-      <c r="F80" s="212"/>
+      <c r="C80" s="188"/>
+      <c r="D80" s="188"/>
+      <c r="E80" s="188"/>
+      <c r="F80" s="188"/>
       <c r="H80" s="61"/>
       <c r="I80" s="61"/>
     </row>
     <row r="81" spans="2:18">
-      <c r="B81" s="200" t="s">
+      <c r="B81" s="211" t="s">
         <v>83</v>
       </c>
       <c r="C81" s="94" t="s">
@@ -4704,7 +4692,7 @@
       <c r="I81" s="61"/>
     </row>
     <row r="82" spans="2:18">
-      <c r="B82" s="201"/>
+      <c r="B82" s="212"/>
       <c r="C82" s="63" t="s">
         <v>66</v>
       </c>
@@ -4724,7 +4712,7 @@
       <c r="I82" s="61"/>
     </row>
     <row r="83" spans="2:18">
-      <c r="B83" s="201"/>
+      <c r="B83" s="212"/>
       <c r="C83" s="63" t="s">
         <v>115</v>
       </c>
@@ -4744,7 +4732,7 @@
       <c r="I83" s="61"/>
     </row>
     <row r="84" spans="2:18">
-      <c r="B84" s="201"/>
+      <c r="B84" s="212"/>
       <c r="C84" s="63" t="s">
         <v>86</v>
       </c>
@@ -4761,7 +4749,7 @@
       <c r="I84" s="61"/>
     </row>
     <row r="85" spans="2:18">
-      <c r="B85" s="201"/>
+      <c r="B85" s="212"/>
       <c r="C85" s="62" t="s">
         <v>64</v>
       </c>
@@ -4778,7 +4766,7 @@
       <c r="I85" s="61"/>
     </row>
     <row r="86" spans="2:18" ht="15" thickBot="1">
-      <c r="B86" s="203"/>
+      <c r="B86" s="214"/>
       <c r="C86" s="69" t="s">
         <v>68</v>
       </c>
@@ -4804,15 +4792,15 @@
     </row>
     <row r="88" spans="2:18" ht="15" thickBot="1">
       <c r="B88" s="59"/>
-      <c r="C88" s="212"/>
-      <c r="D88" s="212"/>
-      <c r="E88" s="212"/>
-      <c r="F88" s="212"/>
+      <c r="C88" s="188"/>
+      <c r="D88" s="188"/>
+      <c r="E88" s="188"/>
+      <c r="F88" s="188"/>
       <c r="H88" s="61"/>
       <c r="I88" s="61"/>
     </row>
     <row r="89" spans="2:18">
-      <c r="B89" s="204" t="s">
+      <c r="B89" s="203" t="s">
         <v>84</v>
       </c>
       <c r="C89" s="113" t="s">
@@ -4834,7 +4822,7 @@
       <c r="I89" s="61"/>
     </row>
     <row r="90" spans="2:18">
-      <c r="B90" s="205"/>
+      <c r="B90" s="215"/>
       <c r="C90" s="66" t="s">
         <v>111</v>
       </c>
@@ -4854,7 +4842,7 @@
       <c r="I90" s="61"/>
     </row>
     <row r="91" spans="2:18">
-      <c r="B91" s="205"/>
+      <c r="B91" s="215"/>
       <c r="C91" s="66" t="s">
         <v>109</v>
       </c>
@@ -4873,8 +4861,8 @@
       <c r="H91" s="61"/>
       <c r="I91" s="61"/>
     </row>
-    <row r="92" spans="2:18" ht="24">
-      <c r="B92" s="205"/>
+    <row r="92" spans="2:18" ht="23">
+      <c r="B92" s="215"/>
       <c r="C92" s="105" t="s">
         <v>166</v>
       </c>
@@ -4894,7 +4882,7 @@
       <c r="I92" s="61"/>
     </row>
     <row r="93" spans="2:18">
-      <c r="B93" s="205"/>
+      <c r="B93" s="215"/>
       <c r="C93" s="66" t="s">
         <v>113</v>
       </c>
@@ -4914,7 +4902,7 @@
       <c r="I93" s="59"/>
       <c r="J93" s="61"/>
       <c r="K93" s="61"/>
-      <c r="L93" s="213"/>
+      <c r="L93" s="189"/>
       <c r="M93" s="59"/>
       <c r="N93" s="59"/>
       <c r="O93" s="59"/>
@@ -4923,7 +4911,7 @@
       <c r="R93" s="4"/>
     </row>
     <row r="94" spans="2:18">
-      <c r="B94" s="205"/>
+      <c r="B94" s="215"/>
       <c r="C94" s="66" t="s">
         <v>86</v>
       </c>
@@ -4941,7 +4929,7 @@
       <c r="I94" s="59"/>
       <c r="J94" s="61"/>
       <c r="K94" s="61"/>
-      <c r="L94" s="213"/>
+      <c r="L94" s="189"/>
       <c r="M94" s="59"/>
       <c r="N94" s="59"/>
       <c r="O94" s="59"/>
@@ -4950,7 +4938,7 @@
       <c r="R94" s="4"/>
     </row>
     <row r="95" spans="2:18">
-      <c r="B95" s="205"/>
+      <c r="B95" s="215"/>
       <c r="C95" s="64" t="s">
         <v>64</v>
       </c>
@@ -4968,7 +4956,7 @@
       <c r="I95" s="60"/>
       <c r="J95" s="61"/>
       <c r="K95" s="61"/>
-      <c r="L95" s="213"/>
+      <c r="L95" s="189"/>
       <c r="M95" s="59"/>
       <c r="N95" s="59"/>
       <c r="O95" s="59"/>
@@ -4977,7 +4965,7 @@
       <c r="R95" s="4"/>
     </row>
     <row r="96" spans="2:18" ht="15" thickBot="1">
-      <c r="B96" s="206"/>
+      <c r="B96" s="204"/>
       <c r="C96" s="68" t="s">
         <v>68</v>
       </c>
@@ -4995,7 +4983,7 @@
       <c r="I96" s="60"/>
       <c r="J96" s="61"/>
       <c r="K96" s="61"/>
-      <c r="L96" s="213"/>
+      <c r="L96" s="189"/>
       <c r="M96" s="59"/>
       <c r="N96" s="59"/>
       <c r="O96" s="59"/>
@@ -5009,7 +4997,7 @@
       <c r="I97" s="61"/>
       <c r="J97" s="61"/>
       <c r="K97" s="61"/>
-      <c r="L97" s="213"/>
+      <c r="L97" s="189"/>
       <c r="M97" s="59"/>
       <c r="N97" s="59"/>
       <c r="O97" s="59"/>
@@ -5023,7 +5011,7 @@
       <c r="I98" s="61"/>
       <c r="J98" s="61"/>
       <c r="K98" s="61"/>
-      <c r="L98" s="213"/>
+      <c r="L98" s="189"/>
       <c r="M98" s="59"/>
       <c r="N98" s="59"/>
       <c r="O98" s="59"/>
@@ -5042,7 +5030,7 @@
       <c r="I99" s="61"/>
       <c r="J99" s="61"/>
       <c r="K99" s="61"/>
-      <c r="L99" s="213"/>
+      <c r="L99" s="189"/>
       <c r="M99" s="59"/>
       <c r="N99" s="59"/>
       <c r="O99" s="59"/>
@@ -5051,7 +5039,7 @@
       <c r="R99" s="4"/>
     </row>
     <row r="100" spans="2:18" s="72" customFormat="1">
-      <c r="B100" s="197" t="s">
+      <c r="B100" s="208" t="s">
         <v>189</v>
       </c>
       <c r="C100" s="111" t="s">
@@ -5070,7 +5058,7 @@
       <c r="L100" s="71"/>
     </row>
     <row r="101" spans="2:18">
-      <c r="B101" s="198"/>
+      <c r="B101" s="209"/>
       <c r="C101" s="109" t="s">
         <v>168</v>
       </c>
@@ -5089,7 +5077,7 @@
       <c r="O101"/>
     </row>
     <row r="102" spans="2:18">
-      <c r="B102" s="198"/>
+      <c r="B102" s="209"/>
       <c r="C102" s="109" t="s">
         <v>169</v>
       </c>
@@ -5108,7 +5096,7 @@
       <c r="O102"/>
     </row>
     <row r="103" spans="2:18">
-      <c r="B103" s="198"/>
+      <c r="B103" s="209"/>
       <c r="C103" s="109" t="s">
         <v>170</v>
       </c>
@@ -5127,7 +5115,7 @@
       <c r="O103"/>
     </row>
     <row r="104" spans="2:18">
-      <c r="B104" s="198"/>
+      <c r="B104" s="209"/>
       <c r="C104" s="109" t="s">
         <v>174</v>
       </c>
@@ -5144,7 +5132,7 @@
       <c r="M104" s="51"/>
     </row>
     <row r="105" spans="2:18">
-      <c r="B105" s="198"/>
+      <c r="B105" s="209"/>
       <c r="C105" s="109" t="s">
         <v>171</v>
       </c>
@@ -5158,7 +5146,7 @@
       <c r="H105" s="53"/>
     </row>
     <row r="106" spans="2:18">
-      <c r="B106" s="198"/>
+      <c r="B106" s="209"/>
       <c r="C106" s="109" t="s">
         <v>172</v>
       </c>
@@ -5170,7 +5158,7 @@
       </c>
     </row>
     <row r="107" spans="2:18">
-      <c r="B107" s="198"/>
+      <c r="B107" s="209"/>
       <c r="C107" s="109" t="s">
         <v>177</v>
       </c>
@@ -5182,7 +5170,7 @@
       </c>
     </row>
     <row r="108" spans="2:18">
-      <c r="B108" s="198"/>
+      <c r="B108" s="209"/>
       <c r="C108" s="109" t="s">
         <v>173</v>
       </c>
@@ -5192,7 +5180,7 @@
       </c>
     </row>
     <row r="109" spans="2:18">
-      <c r="B109" s="198"/>
+      <c r="B109" s="209"/>
       <c r="C109" s="109" t="s">
         <v>182</v>
       </c>
@@ -5204,7 +5192,7 @@
       </c>
     </row>
     <row r="110" spans="2:18" ht="15" thickBot="1">
-      <c r="B110" s="199"/>
+      <c r="B110" s="210"/>
       <c r="C110" s="112" t="s">
         <v>180</v>
       </c>
@@ -5300,18 +5288,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C80:F80"/>
-    <mergeCell ref="C88:F88"/>
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="L93:L99"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B16:B36"/>
-    <mergeCell ref="B37:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B56:B57"/>
     <mergeCell ref="B68:B70"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B100:B110"/>
@@ -5321,6 +5297,18 @@
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B16:B36"/>
+    <mergeCell ref="B37:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C80:F80"/>
+    <mergeCell ref="C88:F88"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="L93:L99"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D68:E68"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5336,25 +5324,25 @@
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1"/>
     <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="218" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="224"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="220"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="225" t="s">
+      <c r="B3" s="221" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="118" t="s">
@@ -5368,7 +5356,7 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="226"/>
+      <c r="B4" s="222"/>
       <c r="C4" s="64" t="s">
         <v>193</v>
       </c>
@@ -5378,7 +5366,7 @@
       <c r="E4" s="67"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="226"/>
+      <c r="B5" s="222"/>
       <c r="C5" s="64" t="s">
         <v>195</v>
       </c>
@@ -5388,7 +5376,7 @@
       <c r="E5" s="67"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="226"/>
+      <c r="B6" s="222"/>
       <c r="C6" s="64" t="s">
         <v>197</v>
       </c>
@@ -5398,7 +5386,7 @@
       <c r="E6" s="67"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="226"/>
+      <c r="B7" s="222"/>
       <c r="C7" s="64" t="s">
         <v>198</v>
       </c>
@@ -5408,7 +5396,7 @@
       <c r="E7" s="67"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="226"/>
+      <c r="B8" s="222"/>
       <c r="C8" s="64" t="s">
         <v>205</v>
       </c>
@@ -5416,7 +5404,7 @@
       <c r="E8" s="67"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="226"/>
+      <c r="B9" s="222"/>
       <c r="C9" s="64" t="s">
         <v>206</v>
       </c>
@@ -5424,7 +5412,7 @@
       <c r="E9" s="67"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="226"/>
+      <c r="B10" s="222"/>
       <c r="C10" s="64" t="s">
         <v>200</v>
       </c>
@@ -5432,7 +5420,7 @@
       <c r="E10" s="88"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="226"/>
+      <c r="B11" s="222"/>
       <c r="C11" s="64" t="s">
         <v>72</v>
       </c>
@@ -5442,7 +5430,7 @@
       <c r="E11" s="88"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="226"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="119" t="s">
         <v>214</v>
       </c>
@@ -5452,7 +5440,7 @@
       <c r="E12" s="89"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="226"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="119" t="s">
         <v>216</v>
       </c>
@@ -5460,7 +5448,7 @@
       <c r="E13" s="89"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="226"/>
+      <c r="B14" s="222"/>
       <c r="C14" s="119" t="s">
         <v>217</v>
       </c>
@@ -5468,7 +5456,7 @@
       <c r="E14" s="89"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="226"/>
+      <c r="B15" s="222"/>
       <c r="C15" s="119" t="s">
         <v>218</v>
       </c>
@@ -5478,7 +5466,7 @@
       <c r="E15" s="89"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="226"/>
+      <c r="B16" s="222"/>
       <c r="C16" s="119" t="s">
         <v>219</v>
       </c>
@@ -5486,7 +5474,7 @@
       <c r="E16" s="89"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="226"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="119" t="s">
         <v>220</v>
       </c>
@@ -5494,7 +5482,7 @@
       <c r="E17" s="65"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="226"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="119" t="s">
         <v>221</v>
       </c>
@@ -5504,7 +5492,7 @@
       <c r="E18" s="65"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="226"/>
+      <c r="B19" s="222"/>
       <c r="C19" s="120" t="s">
         <v>210</v>
       </c>
@@ -5514,7 +5502,7 @@
       <c r="E19" s="65"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="226"/>
+      <c r="B20" s="222"/>
       <c r="C20" s="120" t="s">
         <v>208</v>
       </c>
@@ -5526,7 +5514,7 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="226"/>
+      <c r="B21" s="222"/>
       <c r="C21" s="120" t="s">
         <v>211</v>
       </c>
@@ -5536,7 +5524,7 @@
       <c r="E21" s="65"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="226"/>
+      <c r="B22" s="222"/>
       <c r="C22" s="120" t="s">
         <v>208</v>
       </c>
@@ -5546,7 +5534,7 @@
       <c r="E22" s="65"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="226"/>
+      <c r="B23" s="222"/>
       <c r="C23" s="120" t="s">
         <v>212</v>
       </c>
@@ -5556,7 +5544,7 @@
       <c r="E23" s="67"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="226"/>
+      <c r="B24" s="222"/>
       <c r="C24" s="120" t="s">
         <v>208</v>
       </c>
@@ -5566,7 +5554,7 @@
       <c r="E24" s="67"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="226"/>
+      <c r="B25" s="222"/>
       <c r="C25" s="120" t="s">
         <v>213</v>
       </c>
@@ -5576,7 +5564,7 @@
       <c r="E25" s="67"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="226"/>
+      <c r="B26" s="222"/>
       <c r="C26" s="120" t="s">
         <v>208</v>
       </c>
@@ -5586,7 +5574,7 @@
       <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15" thickBot="1">
-      <c r="B27" s="226"/>
+      <c r="B27" s="222"/>
       <c r="C27" s="121" t="s">
         <v>222</v>
       </c>
@@ -5595,8 +5583,8 @@
       </c>
       <c r="E27" s="102"/>
     </row>
-    <row r="28" spans="2:5" ht="14.45" customHeight="1">
-      <c r="B28" s="227" t="s">
+    <row r="28" spans="2:5" ht="14.5" customHeight="1">
+      <c r="B28" s="223" t="s">
         <v>148</v>
       </c>
       <c r="C28" s="126" t="s">
@@ -5607,8 +5595,8 @@
       </c>
       <c r="E28" s="87"/>
     </row>
-    <row r="29" spans="2:5" ht="14.45" customHeight="1">
-      <c r="B29" s="228"/>
+    <row r="29" spans="2:5" ht="14.5" customHeight="1">
+      <c r="B29" s="224"/>
       <c r="C29" s="78" t="s">
         <v>126</v>
       </c>
@@ -5618,7 +5606,7 @@
       <c r="E29" s="67"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="228"/>
+      <c r="B30" s="224"/>
       <c r="C30" s="78" t="s">
         <v>124</v>
       </c>
@@ -5628,7 +5616,7 @@
       <c r="E30" s="67"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="228"/>
+      <c r="B31" s="224"/>
       <c r="C31" s="78" t="s">
         <v>129</v>
       </c>
@@ -5638,7 +5626,7 @@
       <c r="E31" s="122"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="228"/>
+      <c r="B32" s="224"/>
       <c r="C32" s="78" t="s">
         <v>138</v>
       </c>
@@ -5648,7 +5636,7 @@
       <c r="E32" s="122"/>
     </row>
     <row r="33" spans="2:5" ht="15" thickBot="1">
-      <c r="B33" s="229"/>
+      <c r="B33" s="225"/>
       <c r="C33" s="127" t="s">
         <v>130</v>
       </c>
@@ -5658,7 +5646,7 @@
       <c r="E33" s="129"/>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="225" t="s">
+      <c r="B34" s="221" t="s">
         <v>227</v>
       </c>
       <c r="C34" s="133" t="s">
@@ -5670,7 +5658,7 @@
       <c r="E34" s="130"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="226"/>
+      <c r="B35" s="222"/>
       <c r="C35" s="134" t="s">
         <v>224</v>
       </c>
@@ -5680,7 +5668,7 @@
       <c r="E35" s="67"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="226"/>
+      <c r="B36" s="222"/>
       <c r="C36" s="134" t="s">
         <v>228</v>
       </c>
@@ -5690,7 +5678,7 @@
       <c r="E36" s="67"/>
     </row>
     <row r="37" spans="2:5" ht="15" thickBot="1">
-      <c r="B37" s="230"/>
+      <c r="B37" s="226"/>
       <c r="C37" s="135" t="s">
         <v>226</v>
       </c>
@@ -5700,7 +5688,7 @@
       <c r="E37" s="92"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="204" t="s">
+      <c r="B38" s="203" t="s">
         <v>229</v>
       </c>
       <c r="C38" s="113" t="s">
@@ -5712,27 +5700,27 @@
       <c r="E38" s="87"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="205"/>
+      <c r="B39" s="215"/>
       <c r="C39" s="136" t="s">
         <v>233</v>
       </c>
-      <c r="D39" s="214" t="s">
+      <c r="D39" s="190" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="215"/>
+      <c r="E39" s="191"/>
     </row>
     <row r="40" spans="2:5" ht="15" thickBot="1">
-      <c r="B40" s="205"/>
+      <c r="B40" s="215"/>
       <c r="C40" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="D40" s="220" t="s">
+      <c r="D40" s="216" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="221"/>
+      <c r="E40" s="217"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="207" t="s">
+      <c r="B41" s="196" t="s">
         <v>157</v>
       </c>
       <c r="C41" s="93" t="s">
@@ -5744,7 +5732,7 @@
       <c r="E41" s="98"/>
     </row>
     <row r="42" spans="2:5" ht="15" thickBot="1">
-      <c r="B42" s="209"/>
+      <c r="B42" s="198"/>
       <c r="C42" s="95" t="s">
         <v>156</v>
       </c>
@@ -5780,22 +5768,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40.15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="48.5" customWidth="1"/>
-    <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="48.453125" customWidth="1"/>
+    <col min="4" max="4" width="36.453125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B1" s="232" t="s">
+      <c r="B1" s="228" t="s">
         <v>367</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
     </row>
     <row r="2" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B2" s="197" t="s">
+      <c r="B2" s="208" t="s">
         <v>189</v>
       </c>
       <c r="C2" s="111" t="s">
@@ -5807,17 +5795,17 @@
       <c r="E2" s="87"/>
     </row>
     <row r="3" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B3" s="198"/>
+      <c r="B3" s="209"/>
       <c r="C3" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="153" t="s">
+      <c r="D3" s="151" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B4" s="198"/>
+      <c r="B4" s="209"/>
       <c r="C4" s="109" t="s">
         <v>327</v>
       </c>
@@ -5827,11 +5815,11 @@
       <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B5" s="198"/>
+      <c r="B5" s="209"/>
       <c r="C5" s="109" t="s">
         <v>170</v>
       </c>
-      <c r="D5" s="152">
+      <c r="D5" s="150">
         <v>43921</v>
       </c>
       <c r="E5" s="67" t="s">
@@ -5839,7 +5827,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B6" s="198"/>
+      <c r="B6" s="209"/>
       <c r="C6" s="109" t="s">
         <v>174</v>
       </c>
@@ -5850,44 +5838,44 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B7" s="198"/>
+    <row r="7" spans="1:5" ht="17.5" customHeight="1">
+      <c r="B7" s="209"/>
       <c r="C7" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="152">
+      <c r="D7" s="150">
         <v>43922</v>
       </c>
       <c r="E7" s="67" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B8" s="198"/>
+    <row r="8" spans="1:5" ht="17.5" customHeight="1">
+      <c r="B8" s="209"/>
       <c r="C8" s="109" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="152">
+      <c r="D8" s="150">
         <v>44012</v>
       </c>
       <c r="E8" s="67" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B9" s="198"/>
+    <row r="9" spans="1:5" ht="17.5" customHeight="1">
+      <c r="B9" s="209"/>
       <c r="C9" s="109" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="152" t="s">
+      <c r="D9" s="150" t="s">
         <v>179</v>
       </c>
       <c r="E9" s="67" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B10" s="198"/>
+    <row r="10" spans="1:5" ht="17.5" customHeight="1">
+      <c r="B10" s="209"/>
       <c r="C10" s="109" t="s">
         <v>173</v>
       </c>
@@ -5896,8 +5884,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B11" s="198"/>
+    <row r="11" spans="1:5" ht="17.5" customHeight="1">
+      <c r="B11" s="209"/>
       <c r="C11" s="109" t="s">
         <v>182</v>
       </c>
@@ -5908,8 +5896,8 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
-      <c r="B12" s="199"/>
+    <row r="12" spans="1:5" ht="17.5" customHeight="1" thickBot="1">
+      <c r="B12" s="210"/>
       <c r="C12" s="112" t="s">
         <v>180</v>
       </c>
@@ -5918,14 +5906,14 @@
       </c>
       <c r="E12" s="92"/>
     </row>
-    <row r="13" spans="1:5" ht="17.45" customHeight="1"/>
-    <row r="14" spans="1:5" ht="17.45" customHeight="1"/>
+    <row r="13" spans="1:5" ht="17.5" customHeight="1"/>
+    <row r="14" spans="1:5" ht="17.5" customHeight="1"/>
     <row r="15" spans="1:5" ht="40.15" customHeight="1">
-      <c r="A15" s="231" t="s">
+      <c r="A15" s="227" t="s">
         <v>326</v>
       </c>
-      <c r="B15" s="231"/>
-      <c r="C15" s="231"/>
+      <c r="B15" s="227"/>
+      <c r="C15" s="227"/>
     </row>
     <row r="16" spans="1:5" ht="40.15" customHeight="1">
       <c r="A16" s="139" t="s">
@@ -6143,25 +6131,25 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="52.9" customHeight="1" thickBot="1">
-      <c r="A1" s="180"/>
-      <c r="B1" s="233" t="s">
+      <c r="A1" s="176"/>
+      <c r="B1" s="229" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="234"/>
-      <c r="D1" s="234"/>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
-      <c r="G1" s="234"/>
-      <c r="H1" s="234"/>
-      <c r="I1" s="234"/>
-      <c r="J1" s="234"/>
-      <c r="K1" s="234"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="230"/>
+      <c r="I1" s="230"/>
+      <c r="J1" s="230"/>
+      <c r="K1" s="230"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -6169,44 +6157,44 @@
     </row>
     <row r="2" spans="1:15" ht="52.9" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="177" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="182" t="s">
+      <c r="C2" s="178" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="182" t="s">
+      <c r="D2" s="178" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="182" t="s">
+      <c r="E2" s="178" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="182" t="s">
+      <c r="F2" s="178" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="182" t="s">
+      <c r="G2" s="178" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="182" t="s">
+      <c r="H2" s="178" t="s">
         <v>172</v>
       </c>
-      <c r="I2" s="182" t="s">
+      <c r="I2" s="178" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="182" t="s">
+      <c r="J2" s="178" t="s">
         <v>182</v>
       </c>
-      <c r="K2" s="183" t="s">
+      <c r="K2" s="179" t="s">
         <v>180</v>
       </c>
-      <c r="L2" s="186" t="s">
+      <c r="L2" s="182" t="s">
         <v>370</v>
       </c>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:15" ht="52.9" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="180" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="81"/>
@@ -6223,7 +6211,7 @@
     </row>
     <row r="4" spans="1:15" ht="52.9" customHeight="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="180" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="81"/>
@@ -6240,7 +6228,7 @@
     </row>
     <row r="5" spans="1:15" ht="52.9" customHeight="1" thickBot="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="185" t="s">
+      <c r="B5" s="181" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="97"/>
@@ -6265,30 +6253,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="C35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="29.625" customWidth="1"/>
-    <col min="7" max="7" width="31.5" customWidth="1"/>
-    <col min="8" max="8" width="25.125" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="7" max="7" width="31.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.08984375" customWidth="1"/>
+    <col min="9" max="9" width="30.453125" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5">
-      <c r="A1" s="240" t="s">
+    <row r="1" spans="1:12" ht="26">
+      <c r="A1" s="236" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
     </row>
     <row r="2" spans="1:12" ht="24" thickBot="1">
       <c r="A2" s="145"/>
@@ -6300,23 +6288,23 @@
         <v>240</v>
       </c>
       <c r="E2" s="145"/>
-      <c r="G2" s="237" t="s">
+      <c r="G2" s="233" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="237"/>
-      <c r="I2" s="179" t="s">
+      <c r="H2" s="233"/>
+      <c r="I2" s="175" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1">
       <c r="A3" s="148"/>
-      <c r="B3" s="241" t="s">
+      <c r="B3" s="237" t="s">
         <v>286</v>
       </c>
-      <c r="C3" s="156">
+      <c r="C3" s="154">
         <v>101</v>
       </c>
-      <c r="D3" s="157" t="s">
+      <c r="D3" s="155" t="s">
         <v>251</v>
       </c>
       <c r="E3" s="148"/>
@@ -6327,520 +6315,486 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="35.450000000000003" customHeight="1" thickBot="1">
+    <row r="4" spans="1:12" ht="35.5" customHeight="1" thickBot="1">
       <c r="A4" s="148"/>
-      <c r="B4" s="241"/>
-      <c r="C4" s="156">
+      <c r="B4" s="237"/>
+      <c r="C4" s="154">
         <v>103</v>
       </c>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="155" t="s">
         <v>287</v>
       </c>
       <c r="E4" s="148"/>
-      <c r="G4" s="163" t="s">
+      <c r="G4" s="159" t="s">
         <v>329</v>
       </c>
-      <c r="H4" s="164" t="s">
+      <c r="H4" s="160" t="s">
         <v>339</v>
       </c>
-      <c r="I4" s="238" t="s">
+      <c r="I4" s="234" t="s">
         <v>331</v>
       </c>
-      <c r="K4" s="154"/>
-      <c r="L4" s="154"/>
-    </row>
-    <row r="5" spans="1:12" ht="90.75" thickBot="1">
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+    </row>
+    <row r="5" spans="1:12" ht="93" thickBot="1">
       <c r="A5" s="148"/>
-      <c r="B5" s="241"/>
-      <c r="C5" s="156">
+      <c r="B5" s="237"/>
+      <c r="C5" s="154">
         <v>105</v>
       </c>
-      <c r="D5" s="157" t="s">
+      <c r="D5" s="155" t="s">
         <v>288</v>
       </c>
       <c r="E5" s="148"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="166" t="s">
+      <c r="G5" s="161"/>
+      <c r="H5" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="239"/>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" thickBot="1">
+      <c r="I5" s="235"/>
+    </row>
+    <row r="6" spans="1:12" ht="19" thickBot="1">
       <c r="A6" s="148"/>
-      <c r="B6" s="241"/>
-      <c r="C6" s="156">
+      <c r="B6" s="237"/>
+      <c r="C6" s="154">
         <v>107</v>
       </c>
-      <c r="D6" s="157" t="s">
+      <c r="D6" s="155" t="s">
         <v>289</v>
       </c>
       <c r="E6" s="148"/>
-      <c r="G6" s="165" t="s">
+      <c r="G6" s="161" t="s">
         <v>330</v>
       </c>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="163" t="s">
         <v>333</v>
       </c>
-      <c r="I6" s="161" t="s">
+      <c r="I6" s="157" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75" thickBot="1">
+    <row r="7" spans="1:12" ht="19" thickBot="1">
       <c r="A7" s="148"/>
-      <c r="B7" s="241"/>
-      <c r="C7" s="156">
+      <c r="B7" s="237"/>
+      <c r="C7" s="154">
         <v>109</v>
       </c>
-      <c r="D7" s="157" t="s">
+      <c r="D7" s="155" t="s">
         <v>290</v>
       </c>
       <c r="E7" s="148"/>
-      <c r="G7" s="165" t="s">
+      <c r="G7" s="161" t="s">
         <v>369</v>
       </c>
-      <c r="H7" s="167" t="s">
+      <c r="H7" s="163" t="s">
         <v>334</v>
       </c>
-      <c r="I7" s="161" t="s">
+      <c r="I7" s="157" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="72.75" thickBot="1">
+    <row r="8" spans="1:12" ht="56" thickBot="1">
       <c r="A8" s="148"/>
-      <c r="B8" s="241"/>
-      <c r="C8" s="156">
+      <c r="B8" s="237"/>
+      <c r="C8" s="154">
         <v>111</v>
       </c>
-      <c r="D8" s="157" t="s">
+      <c r="D8" s="155" t="s">
         <v>291</v>
       </c>
       <c r="E8" s="148"/>
-      <c r="G8" s="168" t="s">
+      <c r="G8" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="H8" s="169" t="s">
+      <c r="H8" s="165" t="s">
         <v>338</v>
       </c>
-      <c r="I8" s="162" t="s">
+      <c r="I8" s="158" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1">
       <c r="A9" s="148"/>
-      <c r="B9" s="241"/>
-      <c r="C9" s="156">
+      <c r="B9" s="237"/>
+      <c r="C9" s="154">
         <v>113</v>
       </c>
-      <c r="D9" s="157" t="s">
+      <c r="D9" s="155" t="s">
         <v>292</v>
       </c>
       <c r="E9" s="148"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1">
       <c r="A10" s="148"/>
-      <c r="B10" s="241"/>
-      <c r="C10" s="156">
+      <c r="B10" s="237"/>
+      <c r="C10" s="154">
         <v>115</v>
       </c>
-      <c r="D10" s="157" t="s">
+      <c r="D10" s="155" t="s">
         <v>293</v>
       </c>
       <c r="E10" s="148"/>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1">
       <c r="A11" s="148"/>
-      <c r="B11" s="241"/>
-      <c r="C11" s="156">
+      <c r="B11" s="237"/>
+      <c r="C11" s="154">
         <v>117</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="155" t="s">
         <v>294</v>
       </c>
       <c r="E11" s="148"/>
     </row>
     <row r="12" spans="1:12" ht="70.900000000000006" customHeight="1" thickBot="1">
       <c r="A12" s="148"/>
-      <c r="B12" s="241"/>
-      <c r="C12" s="156">
+      <c r="B12" s="237"/>
+      <c r="C12" s="154">
         <v>119</v>
       </c>
-      <c r="D12" s="157" t="s">
+      <c r="D12" s="155" t="s">
         <v>295</v>
       </c>
       <c r="E12" s="148"/>
     </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1" thickBot="1">
+    <row r="13" spans="1:12" ht="15" thickBot="1">
       <c r="A13" s="148"/>
-      <c r="B13" s="149"/>
-      <c r="C13" s="149"/>
-      <c r="D13" s="150"/>
+      <c r="B13" s="238" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="154">
+        <v>201</v>
+      </c>
+      <c r="D13" s="155" t="s">
+        <v>297</v>
+      </c>
       <c r="E13" s="148"/>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1">
+    <row r="14" spans="1:12" ht="23.5" thickBot="1">
       <c r="A14" s="148"/>
-      <c r="B14" s="242" t="s">
-        <v>296</v>
-      </c>
-      <c r="C14" s="156">
-        <v>201</v>
-      </c>
-      <c r="D14" s="157" t="s">
-        <v>297</v>
+      <c r="B14" s="231"/>
+      <c r="C14" s="154">
+        <v>203</v>
+      </c>
+      <c r="D14" s="155" t="s">
+        <v>298</v>
       </c>
       <c r="E14" s="148"/>
     </row>
-    <row r="15" spans="1:12" ht="24.75" thickBot="1">
+    <row r="15" spans="1:12" ht="15" thickBot="1">
       <c r="A15" s="148"/>
-      <c r="B15" s="235"/>
-      <c r="C15" s="156">
-        <v>203</v>
-      </c>
-      <c r="D15" s="157" t="s">
-        <v>298</v>
+      <c r="B15" s="231"/>
+      <c r="C15" s="154">
+        <v>205</v>
+      </c>
+      <c r="D15" s="155" t="s">
+        <v>299</v>
       </c>
       <c r="E15" s="148"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1">
       <c r="A16" s="148"/>
-      <c r="B16" s="235"/>
-      <c r="C16" s="156">
-        <v>205</v>
-      </c>
-      <c r="D16" s="157" t="s">
-        <v>299</v>
+      <c r="B16" s="232"/>
+      <c r="C16" s="154">
+        <v>207</v>
+      </c>
+      <c r="D16" s="155" t="s">
+        <v>300</v>
       </c>
       <c r="E16" s="148"/>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="A17" s="148"/>
-      <c r="B17" s="236"/>
-      <c r="C17" s="156">
-        <v>207</v>
-      </c>
-      <c r="D17" s="157" t="s">
-        <v>300</v>
+      <c r="B17" s="238" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="154">
+        <v>301</v>
+      </c>
+      <c r="D17" s="155" t="s">
+        <v>270</v>
       </c>
       <c r="E17" s="148"/>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1">
       <c r="A18" s="148"/>
-      <c r="B18" s="149"/>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159"/>
+      <c r="B18" s="231"/>
+      <c r="C18" s="154">
+        <v>303</v>
+      </c>
+      <c r="D18" s="155" t="s">
+        <v>272</v>
+      </c>
       <c r="E18" s="148"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1">
       <c r="A19" s="148"/>
-      <c r="B19" s="242" t="s">
-        <v>301</v>
-      </c>
-      <c r="C19" s="156">
-        <v>301</v>
-      </c>
-      <c r="D19" s="157" t="s">
-        <v>270</v>
+      <c r="B19" s="231"/>
+      <c r="C19" s="154">
+        <v>305</v>
+      </c>
+      <c r="D19" s="155" t="s">
+        <v>302</v>
       </c>
       <c r="E19" s="148"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1">
       <c r="A20" s="148"/>
-      <c r="B20" s="235"/>
-      <c r="C20" s="156">
+      <c r="B20" s="231"/>
+      <c r="C20" s="154">
+        <v>307</v>
+      </c>
+      <c r="D20" s="155" t="s">
         <v>303</v>
-      </c>
-      <c r="D20" s="157" t="s">
-        <v>272</v>
       </c>
       <c r="E20" s="148"/>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1">
       <c r="A21" s="148"/>
-      <c r="B21" s="235"/>
-      <c r="C21" s="156">
-        <v>305</v>
-      </c>
-      <c r="D21" s="157" t="s">
-        <v>302</v>
+      <c r="B21" s="231"/>
+      <c r="C21" s="154">
+        <v>309</v>
+      </c>
+      <c r="D21" s="155" t="s">
+        <v>304</v>
       </c>
       <c r="E21" s="148"/>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1">
       <c r="A22" s="148"/>
-      <c r="B22" s="235"/>
-      <c r="C22" s="156">
-        <v>307</v>
-      </c>
-      <c r="D22" s="157" t="s">
-        <v>303</v>
+      <c r="B22" s="231"/>
+      <c r="C22" s="154">
+        <v>311</v>
+      </c>
+      <c r="D22" s="155" t="s">
+        <v>305</v>
       </c>
       <c r="E22" s="148"/>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1">
       <c r="A23" s="148"/>
-      <c r="B23" s="235"/>
-      <c r="C23" s="156">
-        <v>309</v>
-      </c>
-      <c r="D23" s="157" t="s">
-        <v>304</v>
+      <c r="B23" s="231"/>
+      <c r="C23" s="154">
+        <v>313</v>
+      </c>
+      <c r="D23" s="155" t="s">
+        <v>306</v>
       </c>
       <c r="E23" s="148"/>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1">
       <c r="A24" s="148"/>
-      <c r="B24" s="235"/>
-      <c r="C24" s="156">
-        <v>311</v>
-      </c>
-      <c r="D24" s="157" t="s">
-        <v>305</v>
+      <c r="B24" s="231"/>
+      <c r="C24" s="154">
+        <v>315</v>
+      </c>
+      <c r="D24" s="155" t="s">
+        <v>307</v>
       </c>
       <c r="E24" s="148"/>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1">
       <c r="A25" s="148"/>
-      <c r="B25" s="235"/>
-      <c r="C25" s="156">
-        <v>313</v>
-      </c>
-      <c r="D25" s="157" t="s">
-        <v>306</v>
+      <c r="B25" s="239" t="s">
+        <v>308</v>
+      </c>
+      <c r="C25" s="154">
+        <v>401</v>
+      </c>
+      <c r="D25" s="155" t="s">
+        <v>309</v>
       </c>
       <c r="E25" s="148"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1">
       <c r="A26" s="148"/>
-      <c r="B26" s="235"/>
-      <c r="C26" s="156">
-        <v>315</v>
-      </c>
-      <c r="D26" s="157" t="s">
-        <v>307</v>
+      <c r="B26" s="240"/>
+      <c r="C26" s="154">
+        <v>403</v>
+      </c>
+      <c r="D26" s="155" t="s">
+        <v>310</v>
       </c>
       <c r="E26" s="148"/>
     </row>
-    <row r="27" spans="1:5" ht="21.6" customHeight="1" thickBot="1">
+    <row r="27" spans="1:5" ht="23.5" thickBot="1">
       <c r="A27" s="148"/>
-      <c r="B27" s="236"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="157"/>
+      <c r="B27" s="240"/>
+      <c r="C27" s="154">
+        <v>405</v>
+      </c>
+      <c r="D27" s="155" t="s">
+        <v>311</v>
+      </c>
       <c r="E27" s="148"/>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1">
       <c r="A28" s="148"/>
-      <c r="B28" s="149"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="159"/>
+      <c r="B28" s="240"/>
+      <c r="C28" s="154">
+        <v>407</v>
+      </c>
+      <c r="D28" s="155" t="s">
+        <v>312</v>
+      </c>
       <c r="E28" s="148"/>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1">
       <c r="A29" s="148"/>
-      <c r="B29" s="243" t="s">
-        <v>308</v>
-      </c>
-      <c r="C29" s="156">
-        <v>401</v>
-      </c>
-      <c r="D29" s="157" t="s">
-        <v>309</v>
+      <c r="B29" s="240"/>
+      <c r="C29" s="154">
+        <v>409</v>
+      </c>
+      <c r="D29" s="155" t="s">
+        <v>313</v>
       </c>
       <c r="E29" s="148"/>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1">
+    <row r="30" spans="1:5" ht="23.5" thickBot="1">
       <c r="A30" s="148"/>
-      <c r="B30" s="244"/>
-      <c r="C30" s="156">
-        <v>403</v>
-      </c>
-      <c r="D30" s="157" t="s">
-        <v>310</v>
+      <c r="B30" s="240"/>
+      <c r="C30" s="154">
+        <v>411</v>
+      </c>
+      <c r="D30" s="155" t="s">
+        <v>314</v>
       </c>
       <c r="E30" s="148"/>
     </row>
-    <row r="31" spans="1:5" ht="24.75" thickBot="1">
+    <row r="31" spans="1:5" ht="15" thickBot="1">
       <c r="A31" s="148"/>
-      <c r="B31" s="244"/>
-      <c r="C31" s="156">
-        <v>405</v>
-      </c>
-      <c r="D31" s="157" t="s">
-        <v>311</v>
+      <c r="B31" s="240"/>
+      <c r="C31" s="154">
+        <v>413</v>
+      </c>
+      <c r="D31" s="155" t="s">
+        <v>315</v>
       </c>
       <c r="E31" s="148"/>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1">
       <c r="A32" s="148"/>
-      <c r="B32" s="244"/>
-      <c r="C32" s="156">
-        <v>407</v>
-      </c>
-      <c r="D32" s="157" t="s">
-        <v>312</v>
+      <c r="B32" s="240"/>
+      <c r="C32" s="154">
+        <v>415</v>
+      </c>
+      <c r="D32" s="155" t="s">
+        <v>316</v>
       </c>
       <c r="E32" s="148"/>
     </row>
     <row r="33" spans="1:5" ht="15" thickBot="1">
       <c r="A33" s="148"/>
-      <c r="B33" s="244"/>
-      <c r="C33" s="156">
-        <v>409</v>
-      </c>
-      <c r="D33" s="157" t="s">
-        <v>313</v>
+      <c r="B33" s="240"/>
+      <c r="C33" s="154">
+        <v>417</v>
+      </c>
+      <c r="D33" s="155" t="s">
+        <v>317</v>
       </c>
       <c r="E33" s="148"/>
     </row>
-    <row r="34" spans="1:5" ht="24.75" thickBot="1">
+    <row r="34" spans="1:5" ht="15" thickBot="1">
       <c r="A34" s="148"/>
-      <c r="B34" s="244"/>
-      <c r="C34" s="156">
-        <v>411</v>
-      </c>
-      <c r="D34" s="157" t="s">
-        <v>314</v>
-      </c>
-      <c r="E34" s="148"/>
+      <c r="B34" s="241"/>
+      <c r="C34" s="154">
+        <v>419</v>
+      </c>
+      <c r="D34" s="155" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1">
       <c r="A35" s="148"/>
-      <c r="B35" s="244"/>
-      <c r="C35" s="156">
-        <v>413</v>
-      </c>
-      <c r="D35" s="157" t="s">
-        <v>315</v>
-      </c>
-      <c r="E35" s="148"/>
+      <c r="B35" s="231" t="s">
+        <v>319</v>
+      </c>
+      <c r="C35" s="154">
+        <v>501</v>
+      </c>
+      <c r="D35" s="155" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1">
       <c r="A36" s="148"/>
-      <c r="B36" s="244"/>
-      <c r="C36" s="156">
-        <v>415</v>
-      </c>
-      <c r="D36" s="157" t="s">
-        <v>316</v>
+      <c r="B36" s="231"/>
+      <c r="C36" s="154">
+        <v>503</v>
+      </c>
+      <c r="D36" s="155" t="s">
+        <v>321</v>
       </c>
       <c r="E36" s="148"/>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1">
+    <row r="37" spans="1:5" ht="23.5" thickBot="1">
       <c r="A37" s="148"/>
-      <c r="B37" s="244"/>
-      <c r="C37" s="156">
-        <v>417</v>
-      </c>
-      <c r="D37" s="157" t="s">
-        <v>317</v>
+      <c r="B37" s="231"/>
+      <c r="C37" s="154">
+        <v>505</v>
+      </c>
+      <c r="D37" s="155" t="s">
+        <v>322</v>
       </c>
       <c r="E37" s="148"/>
     </row>
     <row r="38" spans="1:5" ht="15" thickBot="1">
       <c r="A38" s="148"/>
-      <c r="B38" s="245"/>
-      <c r="C38" s="156">
-        <v>419</v>
-      </c>
-      <c r="D38" s="157" t="s">
-        <v>318</v>
+      <c r="B38" s="231"/>
+      <c r="C38" s="154">
+        <v>507</v>
+      </c>
+      <c r="D38" s="155" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1">
       <c r="A39" s="148"/>
-      <c r="C39" s="158"/>
-      <c r="D39" s="159"/>
+      <c r="B39" s="231"/>
+      <c r="C39" s="154">
+        <v>509</v>
+      </c>
+      <c r="D39" s="155" t="s">
+        <v>324</v>
+      </c>
       <c r="E39" s="148"/>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1">
+    <row r="40" spans="1:5" ht="35" thickBot="1">
       <c r="A40" s="148"/>
-      <c r="B40" s="235" t="s">
-        <v>319</v>
-      </c>
-      <c r="C40" s="156">
-        <v>501</v>
-      </c>
-      <c r="D40" s="157" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1">
+      <c r="B40" s="231"/>
+      <c r="C40" s="154">
+        <v>511</v>
+      </c>
+      <c r="D40" s="155" t="s">
+        <v>277</v>
+      </c>
+      <c r="E40" s="149"/>
+    </row>
+    <row r="41" spans="1:5" ht="23.5" thickBot="1">
       <c r="A41" s="148"/>
-      <c r="B41" s="235"/>
-      <c r="C41" s="156">
-        <v>503</v>
-      </c>
-      <c r="D41" s="157" t="s">
-        <v>321</v>
+      <c r="B41" s="232"/>
+      <c r="C41" s="154">
+        <v>513</v>
+      </c>
+      <c r="D41" s="155" t="s">
+        <v>325</v>
       </c>
       <c r="E41" s="148"/>
     </row>
-    <row r="42" spans="1:5" ht="24.75" thickBot="1">
-      <c r="A42" s="148"/>
-      <c r="B42" s="235"/>
-      <c r="C42" s="156">
-        <v>505</v>
-      </c>
-      <c r="D42" s="157" t="s">
-        <v>322</v>
-      </c>
-      <c r="E42" s="148"/>
-    </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1">
-      <c r="A43" s="148"/>
-      <c r="B43" s="235"/>
-      <c r="C43" s="156">
-        <v>507</v>
-      </c>
-      <c r="D43" s="157" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1">
-      <c r="A44" s="148"/>
-      <c r="B44" s="235"/>
-      <c r="C44" s="156">
-        <v>509</v>
-      </c>
-      <c r="D44" s="157" t="s">
-        <v>324</v>
-      </c>
-      <c r="E44" s="148"/>
-    </row>
-    <row r="45" spans="1:5" ht="24.75" thickBot="1">
-      <c r="A45" s="148"/>
-      <c r="B45" s="235"/>
-      <c r="C45" s="156">
-        <v>511</v>
-      </c>
-      <c r="D45" s="157" t="s">
-        <v>277</v>
-      </c>
-      <c r="E45" s="151"/>
-    </row>
-    <row r="46" spans="1:5" ht="24.75" thickBot="1">
-      <c r="A46" s="148"/>
-      <c r="B46" s="236"/>
-      <c r="C46" s="156">
-        <v>513</v>
-      </c>
-      <c r="D46" s="157" t="s">
-        <v>325</v>
-      </c>
-      <c r="E46" s="148"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="C47" s="160"/>
-      <c r="D47" s="160"/>
+    <row r="42" spans="1:5">
+      <c r="C42" s="156"/>
+      <c r="D42" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="B35:B41"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B3:B12"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="B29:B38"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="B25:B34"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6856,67 +6810,67 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="67.150000000000006" customHeight="1">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="245" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="250" t="s">
+      <c r="B1" s="245"/>
+      <c r="C1" s="245"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.5">
+      <c r="A2" s="246" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="250"/>
-      <c r="C2" s="250"/>
-      <c r="D2" s="250"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.5">
-      <c r="A3" s="175" t="s">
+      <c r="B2" s="246"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="246"/>
+      <c r="E2" s="246"/>
+      <c r="F2" s="246"/>
+    </row>
+    <row r="3" spans="1:6" ht="28">
+      <c r="A3" s="171" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="246" t="s">
+      <c r="B3" s="242" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="246"/>
-      <c r="D3" s="246"/>
-      <c r="E3" s="246"/>
-      <c r="F3" s="246"/>
-    </row>
-    <row r="4" spans="1:6" ht="30">
-      <c r="A4" s="174" t="s">
+      <c r="C3" s="242"/>
+      <c r="D3" s="242"/>
+      <c r="E3" s="242"/>
+      <c r="F3" s="242"/>
+    </row>
+    <row r="4" spans="1:6" ht="31">
+      <c r="A4" s="170" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="247" t="s">
+      <c r="B4" s="243" t="s">
         <v>359</v>
       </c>
-      <c r="C4" s="247"/>
-      <c r="D4" s="247"/>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="243"/>
+      <c r="F4" s="243"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="170" t="s">
+      <c r="A5" s="166" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="171" t="s">
+      <c r="B5" s="167" t="s">
         <v>341</v>
       </c>
-      <c r="C5" s="155" t="s">
+      <c r="C5" s="153" t="s">
         <v>342</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -6925,10 +6879,10 @@
       <c r="E5" s="81" t="s">
         <v>344</v>
       </c>
-      <c r="F5" s="155"/>
-    </row>
-    <row r="6" spans="1:6" ht="42.75">
-      <c r="A6" s="152">
+      <c r="F5" s="153"/>
+    </row>
+    <row r="6" spans="1:6" ht="43.5">
+      <c r="A6" s="150">
         <v>43983</v>
       </c>
       <c r="B6" s="81" t="s">
@@ -6937,16 +6891,16 @@
       <c r="C6" s="81" t="s">
         <v>334</v>
       </c>
-      <c r="D6" s="172" t="s">
+      <c r="D6" s="168" t="s">
         <v>345</v>
       </c>
-      <c r="E6" s="155" t="s">
+      <c r="E6" s="153" t="s">
         <v>176</v>
       </c>
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="152">
+      <c r="A7" s="150">
         <v>43984</v>
       </c>
       <c r="B7" s="81" t="s">
@@ -6964,7 +6918,7 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="152">
+      <c r="A8" s="150">
         <v>43985</v>
       </c>
       <c r="B8" s="81" t="s">
@@ -6982,37 +6936,37 @@
       <c r="F8" s="81"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="153" t="s">
         <v>360</v>
       </c>
-      <c r="B9" s="173" t="s">
+      <c r="B9" s="169" t="s">
         <v>353</v>
       </c>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-    </row>
-    <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="174" t="s">
+      <c r="C9" s="153"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="153"/>
+      <c r="F9" s="153"/>
+    </row>
+    <row r="10" spans="1:6" ht="31">
+      <c r="A10" s="170" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="248" t="s">
+      <c r="B10" s="244" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="248"/>
-      <c r="D10" s="248"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="248"/>
+      <c r="C10" s="244"/>
+      <c r="D10" s="244"/>
+      <c r="E10" s="244"/>
+      <c r="F10" s="244"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="170" t="s">
+      <c r="A11" s="166" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="167" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="155" t="s">
+      <c r="C11" s="153" t="s">
         <v>342</v>
       </c>
       <c r="D11" s="81" t="s">
@@ -7021,10 +6975,10 @@
       <c r="E11" s="81" t="s">
         <v>344</v>
       </c>
-      <c r="F11" s="155"/>
-    </row>
-    <row r="12" spans="1:6" ht="42.75">
-      <c r="A12" s="152">
+      <c r="F11" s="153"/>
+    </row>
+    <row r="12" spans="1:6" ht="43.5">
+      <c r="A12" s="150">
         <v>43983</v>
       </c>
       <c r="B12" s="81" t="s">
@@ -7033,16 +6987,16 @@
       <c r="C12" s="81" t="s">
         <v>334</v>
       </c>
-      <c r="D12" s="172" t="s">
+      <c r="D12" s="168" t="s">
         <v>345</v>
       </c>
-      <c r="E12" s="155" t="s">
+      <c r="E12" s="153" t="s">
         <v>176</v>
       </c>
       <c r="F12" s="81"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="152">
+      <c r="A13" s="150">
         <v>43984</v>
       </c>
       <c r="B13" s="81" t="s">
@@ -7060,7 +7014,7 @@
       <c r="F13" s="81"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="152">
+      <c r="A14" s="150">
         <v>43985</v>
       </c>
       <c r="B14" s="81" t="s">
@@ -7078,28 +7032,28 @@
       <c r="F14" s="81"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="153" t="s">
         <v>361</v>
       </c>
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="169" t="s">
         <v>363</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="155"/>
-      <c r="F15" s="155"/>
-    </row>
-    <row r="16" spans="1:6" ht="18">
-      <c r="A16" s="177" t="s">
+      <c r="C15" s="153"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="153"/>
+      <c r="F15" s="153"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.5">
+      <c r="A16" s="173" t="s">
         <v>362</v>
       </c>
-      <c r="B16" s="178" t="s">
+      <c r="B16" s="174" t="s">
         <v>364</v>
       </c>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7121,99 +7075,99 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="42" customHeight="1">
-      <c r="A1" s="251" t="s">
+      <c r="A1" s="247" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
     </row>
     <row r="2" spans="1:8" ht="42" customHeight="1">
-      <c r="A2" s="252" t="s">
+      <c r="A2" s="248" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="252"/>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-      <c r="E2" s="252"/>
-      <c r="F2" s="252"/>
+      <c r="B2" s="248"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="169" t="s">
         <v>344</v>
       </c>
-      <c r="B3" s="173" t="s">
+      <c r="B3" s="169" t="s">
         <v>371</v>
       </c>
-      <c r="C3" s="173" t="s">
+      <c r="C3" s="169" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="173" t="s">
+      <c r="D3" s="169" t="s">
         <v>372</v>
       </c>
-      <c r="E3" s="173" t="s">
+      <c r="E3" s="169" t="s">
         <v>342</v>
       </c>
-      <c r="F3" s="173" t="s">
+      <c r="F3" s="169" t="s">
         <v>341</v>
       </c>
       <c r="G3" s="72"/>
       <c r="H3" s="72"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="A4" s="190" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="186" t="s">
         <v>376</v>
       </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
       <c r="G4" s="72"/>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="24.6" customHeight="1">
-      <c r="A5" s="173"/>
-      <c r="B5" s="152">
+    <row r="5" spans="1:8" ht="24.65" customHeight="1">
+      <c r="A5" s="169"/>
+      <c r="B5" s="150">
         <v>43983</v>
       </c>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="169" t="s">
         <v>359</v>
       </c>
-      <c r="D5" s="188" t="s">
+      <c r="D5" s="184" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="189" t="s">
+      <c r="E5" s="185" t="s">
         <v>334</v>
       </c>
-      <c r="F5" s="189" t="s">
+      <c r="F5" s="185" t="s">
         <v>333</v>
       </c>
-      <c r="G5" s="187"/>
-      <c r="H5" s="187"/>
-    </row>
-    <row r="6" spans="1:8" ht="56.25">
-      <c r="A6" s="173"/>
-      <c r="B6" s="152">
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+    </row>
+    <row r="6" spans="1:8" ht="52.5">
+      <c r="A6" s="169"/>
+      <c r="B6" s="150">
         <v>43983</v>
       </c>
-      <c r="C6" s="173" t="s">
+      <c r="C6" s="169" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="188" t="s">
+      <c r="D6" s="184" t="s">
         <v>373</v>
       </c>
-      <c r="E6" s="189" t="s">
+      <c r="E6" s="185" t="s">
         <v>334</v>
       </c>
       <c r="F6" s="81" t="s">
@@ -7221,54 +7175,54 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="169" t="s">
         <v>374</v>
       </c>
-      <c r="B7" s="173"/>
-      <c r="C7" s="173"/>
-      <c r="D7" s="173"/>
-      <c r="E7" s="173"/>
-      <c r="F7" s="173" t="s">
+      <c r="B7" s="169"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="191" t="s">
+    <row r="8" spans="1:8" ht="15.5">
+      <c r="A8" s="187" t="s">
         <v>377</v>
       </c>
-      <c r="B8" s="173"/>
-      <c r="C8" s="173"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="173"/>
-      <c r="F8" s="173"/>
-    </row>
-    <row r="9" spans="1:8" ht="56.25">
-      <c r="A9" s="173"/>
-      <c r="B9" s="152">
+      <c r="B8" s="169"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+    </row>
+    <row r="9" spans="1:8" ht="52.5">
+      <c r="A9" s="169"/>
+      <c r="B9" s="150">
         <v>43984</v>
       </c>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="169" t="s">
         <v>175</v>
       </c>
-      <c r="D9" s="188" t="s">
+      <c r="D9" s="184" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="81" t="s">
         <v>348</v>
       </c>
-      <c r="F9" s="189" t="s">
+      <c r="F9" s="185" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56.25">
-      <c r="A10" s="173"/>
-      <c r="B10" s="152">
+    <row r="10" spans="1:8" ht="52.5">
+      <c r="A10" s="169"/>
+      <c r="B10" s="150">
         <v>43985</v>
       </c>
-      <c r="C10" s="173" t="s">
+      <c r="C10" s="169" t="s">
         <v>359</v>
       </c>
-      <c r="D10" s="188" t="s">
+      <c r="D10" s="184" t="s">
         <v>373</v>
       </c>
       <c r="E10" s="81" t="s">
@@ -7279,14 +7233,14 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="169" t="s">
         <v>374</v>
       </c>
-      <c r="B11" s="173"/>
-      <c r="C11" s="173"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="173" t="s">
+      <c r="B11" s="169"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="169"/>
+      <c r="F11" s="169" t="s">
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish corp individual relationship
</commit_message>
<xml_diff>
--- a/zoe_documents/网页设计 zoe.xlsx
+++ b/zoe_documents/网页设计 zoe.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="23040" windowHeight="10935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="23040" windowHeight="10935" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="公司信息" sheetId="1" r:id="rId1"/>
@@ -2993,273 +2993,6 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3288,31 +3021,13 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3327,6 +3042,291 @@
     </xf>
     <xf numFmtId="0" fontId="41" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3365,7 +3365,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8035E939-033C-4405-97D4-C15A2CD78939}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8035E939-033C-4405-97D4-C15A2CD78939}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4123,7 +4123,7 @@
       <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="B16" s="243" t="s">
+      <c r="B16" s="254" t="s">
         <v>154</v>
       </c>
       <c r="C16" s="85" t="s">
@@ -4140,7 +4140,7 @@
       <c r="J16" s="60"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="244"/>
+      <c r="B17" s="255"/>
       <c r="C17" s="84" t="s">
         <v>61</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="J17" s="59"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="244"/>
+      <c r="B18" s="255"/>
       <c r="C18" s="84" t="s">
         <v>62</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="J18" s="59"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="244"/>
+      <c r="B19" s="255"/>
       <c r="C19" s="84" t="s">
         <v>100</v>
       </c>
@@ -4180,7 +4180,7 @@
       <c r="K19" s="58"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="244"/>
+      <c r="B20" s="255"/>
       <c r="C20" s="84" t="s">
         <v>101</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="K20" s="58"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="244"/>
+      <c r="B21" s="255"/>
       <c r="C21" s="77" t="s">
         <v>87</v>
       </c>
@@ -4210,7 +4210,7 @@
       <c r="K21" s="58"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="244"/>
+      <c r="B22" s="255"/>
       <c r="C22" s="77" t="s">
         <v>88</v>
       </c>
@@ -4225,7 +4225,7 @@
       <c r="J22" s="59"/>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="244"/>
+      <c r="B23" s="255"/>
       <c r="C23" s="84" t="s">
         <v>89</v>
       </c>
@@ -4239,7 +4239,7 @@
       <c r="I23" s="61"/>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="244"/>
+      <c r="B24" s="255"/>
       <c r="C24" s="77" t="s">
         <v>92</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="I24" s="61"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="244"/>
+      <c r="B25" s="255"/>
       <c r="C25" s="84" t="s">
         <v>94</v>
       </c>
@@ -4271,7 +4271,7 @@
       <c r="K25" s="110"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="244"/>
+      <c r="B26" s="255"/>
       <c r="C26" s="84" t="s">
         <v>95</v>
       </c>
@@ -4288,7 +4288,7 @@
       <c r="K26" s="59"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="244"/>
+      <c r="B27" s="255"/>
       <c r="C27" s="77" t="s">
         <v>102</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="I27" s="61"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="244"/>
+      <c r="B28" s="255"/>
       <c r="C28" s="77" t="s">
         <v>103</v>
       </c>
@@ -4314,7 +4314,7 @@
       <c r="I28" s="61"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="244"/>
+      <c r="B29" s="255"/>
       <c r="C29" s="84" t="s">
         <v>199</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="I29" s="61"/>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="244"/>
+      <c r="B30" s="255"/>
       <c r="C30" s="84" t="s">
         <v>200</v>
       </c>
@@ -4336,7 +4336,7 @@
       <c r="I30" s="61"/>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="244"/>
+      <c r="B31" s="255"/>
       <c r="C31" s="84" t="s">
         <v>202</v>
       </c>
@@ -4349,7 +4349,7 @@
       <c r="I31" s="61"/>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="244"/>
+      <c r="B32" s="255"/>
       <c r="C32" s="84" t="s">
         <v>203</v>
       </c>
@@ -4360,7 +4360,7 @@
       <c r="I32" s="61"/>
     </row>
     <row r="33" spans="2:9">
-      <c r="B33" s="244"/>
+      <c r="B33" s="255"/>
       <c r="C33" s="84" t="s">
         <v>67</v>
       </c>
@@ -4371,7 +4371,7 @@
       <c r="I33" s="61"/>
     </row>
     <row r="34" spans="2:9">
-      <c r="B34" s="244"/>
+      <c r="B34" s="255"/>
       <c r="C34" s="84" t="s">
         <v>68</v>
       </c>
@@ -4381,7 +4381,7 @@
       <c r="I34" s="61"/>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="244"/>
+      <c r="B35" s="255"/>
       <c r="C35" s="84" t="s">
         <v>69</v>
       </c>
@@ -4391,7 +4391,7 @@
       <c r="I35" s="61"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B36" s="245"/>
+      <c r="B36" s="256"/>
       <c r="C36" s="90" t="s">
         <v>72</v>
       </c>
@@ -4403,7 +4403,7 @@
       <c r="I36" s="61"/>
     </row>
     <row r="37" spans="2:9">
-      <c r="B37" s="231" t="s">
+      <c r="B37" s="257" t="s">
         <v>148</v>
       </c>
       <c r="C37" s="93" t="s">
@@ -4417,7 +4417,7 @@
       <c r="I37" s="61"/>
     </row>
     <row r="38" spans="2:9">
-      <c r="B38" s="246"/>
+      <c r="B38" s="258"/>
       <c r="C38" s="77" t="s">
         <v>126</v>
       </c>
@@ -4429,7 +4429,7 @@
       <c r="I38" s="61"/>
     </row>
     <row r="39" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B39" s="246"/>
+      <c r="B39" s="258"/>
       <c r="C39" s="77" t="s">
         <v>121</v>
       </c>
@@ -4443,7 +4443,7 @@
       <c r="I39" s="61"/>
     </row>
     <row r="40" spans="2:9">
-      <c r="B40" s="246"/>
+      <c r="B40" s="258"/>
       <c r="C40" s="77" t="s">
         <v>135</v>
       </c>
@@ -4455,7 +4455,7 @@
       <c r="I40" s="61"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B41" s="246"/>
+      <c r="B41" s="258"/>
       <c r="C41" s="77" t="s">
         <v>125</v>
       </c>
@@ -4467,7 +4467,7 @@
       <c r="I41" s="61"/>
     </row>
     <row r="42" spans="2:9">
-      <c r="B42" s="246"/>
+      <c r="B42" s="258"/>
       <c r="C42" s="77" t="s">
         <v>136</v>
       </c>
@@ -4479,7 +4479,7 @@
       <c r="I42" s="61"/>
     </row>
     <row r="43" spans="2:9">
-      <c r="B43" s="246"/>
+      <c r="B43" s="258"/>
       <c r="C43" s="77" t="s">
         <v>230</v>
       </c>
@@ -4491,7 +4491,7 @@
       <c r="I43" s="61"/>
     </row>
     <row r="44" spans="2:9">
-      <c r="B44" s="246"/>
+      <c r="B44" s="258"/>
       <c r="C44" s="77" t="s">
         <v>231</v>
       </c>
@@ -4503,7 +4503,7 @@
       <c r="I44" s="61"/>
     </row>
     <row r="45" spans="2:9">
-      <c r="B45" s="246"/>
+      <c r="B45" s="258"/>
       <c r="C45" s="77" t="s">
         <v>232</v>
       </c>
@@ -4515,7 +4515,7 @@
       <c r="I45" s="61"/>
     </row>
     <row r="46" spans="2:9">
-      <c r="B46" s="246"/>
+      <c r="B46" s="258"/>
       <c r="C46" s="77" t="s">
         <v>137</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="I46" s="61"/>
     </row>
     <row r="47" spans="2:9">
-      <c r="B47" s="246"/>
+      <c r="B47" s="258"/>
       <c r="C47" s="77" t="s">
         <v>129</v>
       </c>
@@ -4539,7 +4539,7 @@
       <c r="I47" s="61"/>
     </row>
     <row r="48" spans="2:9">
-      <c r="B48" s="247"/>
+      <c r="B48" s="259"/>
       <c r="C48" s="77" t="s">
         <v>162</v>
       </c>
@@ -4551,7 +4551,7 @@
       <c r="I48" s="61"/>
     </row>
     <row r="49" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B49" s="232"/>
+      <c r="B49" s="260"/>
       <c r="C49" s="95" t="s">
         <v>130</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="I49" s="61"/>
     </row>
     <row r="50" spans="2:9">
-      <c r="B50" s="231" t="s">
+      <c r="B50" s="257" t="s">
         <v>131</v>
       </c>
       <c r="C50" s="93" t="s">
@@ -4577,7 +4577,7 @@
       <c r="I50" s="61"/>
     </row>
     <row r="51" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B51" s="232"/>
+      <c r="B51" s="260"/>
       <c r="C51" s="95" t="s">
         <v>131</v>
       </c>
@@ -4589,7 +4589,7 @@
       <c r="I51" s="61"/>
     </row>
     <row r="52" spans="2:9">
-      <c r="B52" s="231" t="s">
+      <c r="B52" s="257" t="s">
         <v>132</v>
       </c>
       <c r="C52" s="93" t="s">
@@ -4603,7 +4603,7 @@
       <c r="I52" s="61"/>
     </row>
     <row r="53" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B53" s="232"/>
+      <c r="B53" s="260"/>
       <c r="C53" s="95" t="s">
         <v>132</v>
       </c>
@@ -4615,7 +4615,7 @@
       <c r="I53" s="61"/>
     </row>
     <row r="54" spans="2:9">
-      <c r="B54" s="231" t="s">
+      <c r="B54" s="257" t="s">
         <v>163</v>
       </c>
       <c r="C54" s="93" t="s">
@@ -4629,7 +4629,7 @@
       <c r="I54" s="61"/>
     </row>
     <row r="55" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B55" s="232"/>
+      <c r="B55" s="260"/>
       <c r="C55" s="95" t="s">
         <v>165</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="I55" s="61"/>
     </row>
     <row r="56" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B56" s="240" t="s">
+      <c r="B56" s="261" t="s">
         <v>150</v>
       </c>
       <c r="C56" s="93" t="s">
@@ -4655,7 +4655,7 @@
       <c r="I56" s="61"/>
     </row>
     <row r="57" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B57" s="242"/>
+      <c r="B57" s="262"/>
       <c r="C57" s="95" t="s">
         <v>147</v>
       </c>
@@ -4667,7 +4667,7 @@
       <c r="I57" s="61"/>
     </row>
     <row r="58" spans="2:9">
-      <c r="B58" s="243" t="s">
+      <c r="B58" s="254" t="s">
         <v>151</v>
       </c>
       <c r="C58" s="93" t="s">
@@ -4681,31 +4681,31 @@
       <c r="I58" s="61"/>
     </row>
     <row r="59" spans="2:9">
-      <c r="B59" s="244"/>
+      <c r="B59" s="255"/>
       <c r="C59" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="250" t="s">
+      <c r="D59" s="248" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="251"/>
+      <c r="E59" s="249"/>
       <c r="H59" s="61"/>
       <c r="I59" s="61"/>
     </row>
     <row r="60" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B60" s="245"/>
+      <c r="B60" s="256"/>
       <c r="C60" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="252" t="s">
+      <c r="D60" s="250" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="253"/>
+      <c r="E60" s="251"/>
       <c r="H60" s="61"/>
       <c r="I60" s="61"/>
     </row>
     <row r="61" spans="2:9">
-      <c r="B61" s="240" t="s">
+      <c r="B61" s="261" t="s">
         <v>152</v>
       </c>
       <c r="C61" s="93" t="s">
@@ -4719,7 +4719,7 @@
       <c r="I61" s="61"/>
     </row>
     <row r="62" spans="2:9">
-      <c r="B62" s="241"/>
+      <c r="B62" s="273"/>
       <c r="C62" s="77" t="s">
         <v>128</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="I62" s="61"/>
     </row>
     <row r="63" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B63" s="242"/>
+      <c r="B63" s="262"/>
       <c r="C63" s="95" t="s">
         <v>134</v>
       </c>
@@ -4743,7 +4743,7 @@
       <c r="I63" s="61"/>
     </row>
     <row r="64" spans="2:9">
-      <c r="B64" s="243" t="s">
+      <c r="B64" s="254" t="s">
         <v>153</v>
       </c>
       <c r="C64" s="93" t="s">
@@ -4757,7 +4757,7 @@
       <c r="I64" s="61"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="B65" s="244"/>
+      <c r="B65" s="255"/>
       <c r="C65" s="77" t="s">
         <v>145</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="I65" s="61"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="B66" s="244"/>
+      <c r="B66" s="255"/>
       <c r="C66" s="77" t="s">
         <v>142</v>
       </c>
@@ -4781,7 +4781,7 @@
       <c r="I66" s="61"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B67" s="245"/>
+      <c r="B67" s="256"/>
       <c r="C67" s="95" t="s">
         <v>144</v>
       </c>
@@ -4793,21 +4793,21 @@
       <c r="I67" s="61"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="B68" s="228" t="s">
+      <c r="B68" s="263" t="s">
         <v>157</v>
       </c>
       <c r="C68" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="254" t="s">
+      <c r="D68" s="252" t="s">
         <v>118</v>
       </c>
-      <c r="E68" s="255"/>
+      <c r="E68" s="253"/>
       <c r="H68" s="61"/>
       <c r="I68" s="61"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B69" s="229"/>
+      <c r="B69" s="264"/>
       <c r="C69" s="103" t="s">
         <v>167</v>
       </c>
@@ -4819,7 +4819,7 @@
       <c r="I69" s="61"/>
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B70" s="230"/>
+      <c r="B70" s="265"/>
       <c r="C70" s="91" t="s">
         <v>156</v>
       </c>
@@ -4836,16 +4836,16 @@
     </row>
     <row r="72" spans="1:10" ht="15.75" thickBot="1">
       <c r="B72" s="59"/>
-      <c r="C72" s="248"/>
-      <c r="D72" s="248"/>
-      <c r="E72" s="248"/>
-      <c r="F72" s="248"/>
+      <c r="C72" s="246"/>
+      <c r="D72" s="246"/>
+      <c r="E72" s="246"/>
+      <c r="F72" s="246"/>
       <c r="H72" s="61"/>
       <c r="I72" s="61"/>
       <c r="J72" s="59"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="B73" s="236" t="s">
+      <c r="B73" s="269" t="s">
         <v>85</v>
       </c>
       <c r="C73" s="116" t="s">
@@ -4865,7 +4865,7 @@
       <c r="J73" s="59"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="B74" s="237"/>
+      <c r="B74" s="270"/>
       <c r="C74" s="63" t="s">
         <v>143</v>
       </c>
@@ -4883,7 +4883,7 @@
       <c r="J74" s="59"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="B75" s="237"/>
+      <c r="B75" s="270"/>
       <c r="C75" s="63" t="s">
         <v>66</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="I75" s="61"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="B76" s="237"/>
+      <c r="B76" s="270"/>
       <c r="C76" s="62" t="s">
         <v>64</v>
       </c>
@@ -4917,7 +4917,7 @@
       <c r="I76" s="61"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="B77" s="238"/>
+      <c r="B77" s="271"/>
       <c r="C77" s="114" t="s">
         <v>204</v>
       </c>
@@ -4934,7 +4934,7 @@
       <c r="I77" s="61"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B78" s="239"/>
+      <c r="B78" s="272"/>
       <c r="C78" s="69" t="s">
         <v>68</v>
       </c>
@@ -4961,15 +4961,15 @@
         <v>46</v>
       </c>
       <c r="B80" s="59"/>
-      <c r="C80" s="248"/>
-      <c r="D80" s="248"/>
-      <c r="E80" s="248"/>
-      <c r="F80" s="248"/>
+      <c r="C80" s="246"/>
+      <c r="D80" s="246"/>
+      <c r="E80" s="246"/>
+      <c r="F80" s="246"/>
       <c r="H80" s="61"/>
       <c r="I80" s="61"/>
     </row>
     <row r="81" spans="2:18">
-      <c r="B81" s="236" t="s">
+      <c r="B81" s="269" t="s">
         <v>83</v>
       </c>
       <c r="C81" s="94" t="s">
@@ -4991,7 +4991,7 @@
       <c r="I81" s="61"/>
     </row>
     <row r="82" spans="2:18">
-      <c r="B82" s="237"/>
+      <c r="B82" s="270"/>
       <c r="C82" s="63" t="s">
         <v>66</v>
       </c>
@@ -5011,7 +5011,7 @@
       <c r="I82" s="61"/>
     </row>
     <row r="83" spans="2:18">
-      <c r="B83" s="237"/>
+      <c r="B83" s="270"/>
       <c r="C83" s="63" t="s">
         <v>115</v>
       </c>
@@ -5031,7 +5031,7 @@
       <c r="I83" s="61"/>
     </row>
     <row r="84" spans="2:18">
-      <c r="B84" s="237"/>
+      <c r="B84" s="270"/>
       <c r="C84" s="63" t="s">
         <v>86</v>
       </c>
@@ -5048,7 +5048,7 @@
       <c r="I84" s="61"/>
     </row>
     <row r="85" spans="2:18">
-      <c r="B85" s="237"/>
+      <c r="B85" s="270"/>
       <c r="C85" s="62" t="s">
         <v>64</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="I85" s="61"/>
     </row>
     <row r="86" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B86" s="239"/>
+      <c r="B86" s="272"/>
       <c r="C86" s="69" t="s">
         <v>68</v>
       </c>
@@ -5091,15 +5091,15 @@
     </row>
     <row r="88" spans="2:18" ht="15.75" thickBot="1">
       <c r="B88" s="59"/>
-      <c r="C88" s="248"/>
-      <c r="D88" s="248"/>
-      <c r="E88" s="248"/>
-      <c r="F88" s="248"/>
+      <c r="C88" s="246"/>
+      <c r="D88" s="246"/>
+      <c r="E88" s="246"/>
+      <c r="F88" s="246"/>
       <c r="H88" s="61"/>
       <c r="I88" s="61"/>
     </row>
     <row r="89" spans="2:18">
-      <c r="B89" s="240" t="s">
+      <c r="B89" s="261" t="s">
         <v>84</v>
       </c>
       <c r="C89" s="113" t="s">
@@ -5121,7 +5121,7 @@
       <c r="I89" s="61"/>
     </row>
     <row r="90" spans="2:18">
-      <c r="B90" s="241"/>
+      <c r="B90" s="273"/>
       <c r="C90" s="66" t="s">
         <v>111</v>
       </c>
@@ -5141,7 +5141,7 @@
       <c r="I90" s="61"/>
     </row>
     <row r="91" spans="2:18">
-      <c r="B91" s="241"/>
+      <c r="B91" s="273"/>
       <c r="C91" s="66" t="s">
         <v>109</v>
       </c>
@@ -5161,7 +5161,7 @@
       <c r="I91" s="61"/>
     </row>
     <row r="92" spans="2:18" ht="24">
-      <c r="B92" s="241"/>
+      <c r="B92" s="273"/>
       <c r="C92" s="105" t="s">
         <v>166</v>
       </c>
@@ -5181,7 +5181,7 @@
       <c r="I92" s="61"/>
     </row>
     <row r="93" spans="2:18">
-      <c r="B93" s="241"/>
+      <c r="B93" s="273"/>
       <c r="C93" s="66" t="s">
         <v>113</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="I93" s="59"/>
       <c r="J93" s="61"/>
       <c r="K93" s="61"/>
-      <c r="L93" s="249"/>
+      <c r="L93" s="247"/>
       <c r="M93" s="59"/>
       <c r="N93" s="59"/>
       <c r="O93" s="59"/>
@@ -5210,7 +5210,7 @@
       <c r="R93" s="4"/>
     </row>
     <row r="94" spans="2:18">
-      <c r="B94" s="241"/>
+      <c r="B94" s="273"/>
       <c r="C94" s="66" t="s">
         <v>86</v>
       </c>
@@ -5228,7 +5228,7 @@
       <c r="I94" s="59"/>
       <c r="J94" s="61"/>
       <c r="K94" s="61"/>
-      <c r="L94" s="249"/>
+      <c r="L94" s="247"/>
       <c r="M94" s="59"/>
       <c r="N94" s="59"/>
       <c r="O94" s="59"/>
@@ -5237,7 +5237,7 @@
       <c r="R94" s="4"/>
     </row>
     <row r="95" spans="2:18">
-      <c r="B95" s="241"/>
+      <c r="B95" s="273"/>
       <c r="C95" s="64" t="s">
         <v>64</v>
       </c>
@@ -5255,7 +5255,7 @@
       <c r="I95" s="60"/>
       <c r="J95" s="61"/>
       <c r="K95" s="61"/>
-      <c r="L95" s="249"/>
+      <c r="L95" s="247"/>
       <c r="M95" s="59"/>
       <c r="N95" s="59"/>
       <c r="O95" s="59"/>
@@ -5264,7 +5264,7 @@
       <c r="R95" s="4"/>
     </row>
     <row r="96" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B96" s="242"/>
+      <c r="B96" s="262"/>
       <c r="C96" s="68" t="s">
         <v>68</v>
       </c>
@@ -5282,7 +5282,7 @@
       <c r="I96" s="60"/>
       <c r="J96" s="61"/>
       <c r="K96" s="61"/>
-      <c r="L96" s="249"/>
+      <c r="L96" s="247"/>
       <c r="M96" s="59"/>
       <c r="N96" s="59"/>
       <c r="O96" s="59"/>
@@ -5296,7 +5296,7 @@
       <c r="I97" s="61"/>
       <c r="J97" s="61"/>
       <c r="K97" s="61"/>
-      <c r="L97" s="249"/>
+      <c r="L97" s="247"/>
       <c r="M97" s="59"/>
       <c r="N97" s="59"/>
       <c r="O97" s="59"/>
@@ -5310,7 +5310,7 @@
       <c r="I98" s="61"/>
       <c r="J98" s="61"/>
       <c r="K98" s="61"/>
-      <c r="L98" s="249"/>
+      <c r="L98" s="247"/>
       <c r="M98" s="59"/>
       <c r="N98" s="59"/>
       <c r="O98" s="59"/>
@@ -5329,7 +5329,7 @@
       <c r="I99" s="61"/>
       <c r="J99" s="61"/>
       <c r="K99" s="61"/>
-      <c r="L99" s="249"/>
+      <c r="L99" s="247"/>
       <c r="M99" s="59"/>
       <c r="N99" s="59"/>
       <c r="O99" s="59"/>
@@ -5338,7 +5338,7 @@
       <c r="R99" s="4"/>
     </row>
     <row r="100" spans="2:18" s="72" customFormat="1">
-      <c r="B100" s="233" t="s">
+      <c r="B100" s="266" t="s">
         <v>189</v>
       </c>
       <c r="C100" s="111" t="s">
@@ -5357,7 +5357,7 @@
       <c r="L100" s="71"/>
     </row>
     <row r="101" spans="2:18">
-      <c r="B101" s="234"/>
+      <c r="B101" s="267"/>
       <c r="C101" s="109" t="s">
         <v>168</v>
       </c>
@@ -5376,7 +5376,7 @@
       <c r="O101"/>
     </row>
     <row r="102" spans="2:18">
-      <c r="B102" s="234"/>
+      <c r="B102" s="267"/>
       <c r="C102" s="109" t="s">
         <v>169</v>
       </c>
@@ -5395,7 +5395,7 @@
       <c r="O102"/>
     </row>
     <row r="103" spans="2:18">
-      <c r="B103" s="234"/>
+      <c r="B103" s="267"/>
       <c r="C103" s="109" t="s">
         <v>170</v>
       </c>
@@ -5414,7 +5414,7 @@
       <c r="O103"/>
     </row>
     <row r="104" spans="2:18">
-      <c r="B104" s="234"/>
+      <c r="B104" s="267"/>
       <c r="C104" s="109" t="s">
         <v>174</v>
       </c>
@@ -5431,7 +5431,7 @@
       <c r="M104" s="51"/>
     </row>
     <row r="105" spans="2:18">
-      <c r="B105" s="234"/>
+      <c r="B105" s="267"/>
       <c r="C105" s="109" t="s">
         <v>171</v>
       </c>
@@ -5445,7 +5445,7 @@
       <c r="H105" s="53"/>
     </row>
     <row r="106" spans="2:18">
-      <c r="B106" s="234"/>
+      <c r="B106" s="267"/>
       <c r="C106" s="109" t="s">
         <v>172</v>
       </c>
@@ -5457,7 +5457,7 @@
       </c>
     </row>
     <row r="107" spans="2:18">
-      <c r="B107" s="234"/>
+      <c r="B107" s="267"/>
       <c r="C107" s="109" t="s">
         <v>177</v>
       </c>
@@ -5469,7 +5469,7 @@
       </c>
     </row>
     <row r="108" spans="2:18">
-      <c r="B108" s="234"/>
+      <c r="B108" s="267"/>
       <c r="C108" s="109" t="s">
         <v>173</v>
       </c>
@@ -5479,7 +5479,7 @@
       </c>
     </row>
     <row r="109" spans="2:18">
-      <c r="B109" s="234"/>
+      <c r="B109" s="267"/>
       <c r="C109" s="109" t="s">
         <v>182</v>
       </c>
@@ -5491,7 +5491,7 @@
       </c>
     </row>
     <row r="110" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B110" s="235"/>
+      <c r="B110" s="268"/>
       <c r="C110" s="112" t="s">
         <v>180</v>
       </c>
@@ -5587,18 +5587,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C80:F80"/>
-    <mergeCell ref="C88:F88"/>
-    <mergeCell ref="C72:F72"/>
-    <mergeCell ref="L93:L99"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B16:B36"/>
-    <mergeCell ref="B37:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B56:B57"/>
     <mergeCell ref="B68:B70"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B100:B110"/>
@@ -5608,6 +5596,18 @@
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B61:B63"/>
     <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B16:B36"/>
+    <mergeCell ref="B37:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C80:F80"/>
+    <mergeCell ref="C88:F88"/>
+    <mergeCell ref="C72:F72"/>
+    <mergeCell ref="L93:L99"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D68:E68"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5619,7 +5619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -5642,10 +5642,10 @@
       <c r="C1" s="191">
         <v>1</v>
       </c>
-      <c r="D1" s="337" t="s">
+      <c r="D1" s="242" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="338"/>
+      <c r="E1" s="243"/>
       <c r="M1"/>
       <c r="N1"/>
     </row>
@@ -5657,10 +5657,10 @@
       <c r="C2" s="191">
         <v>2</v>
       </c>
-      <c r="D2" s="339" t="s">
+      <c r="D2" s="244" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="338"/>
+      <c r="E2" s="243"/>
       <c r="M2"/>
       <c r="N2"/>
     </row>
@@ -5672,10 +5672,10 @@
       <c r="C3" s="191">
         <v>3</v>
       </c>
-      <c r="D3" s="339" t="s">
+      <c r="D3" s="244" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="338"/>
+      <c r="E3" s="243"/>
       <c r="M3"/>
       <c r="N3"/>
     </row>
@@ -5687,10 +5687,10 @@
       <c r="C4" s="191">
         <v>4</v>
       </c>
-      <c r="D4" s="339" t="s">
+      <c r="D4" s="244" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="338"/>
+      <c r="E4" s="243"/>
       <c r="M4"/>
       <c r="N4"/>
     </row>
@@ -5702,10 +5702,10 @@
       <c r="C5" s="191">
         <v>5</v>
       </c>
-      <c r="D5" s="340" t="s">
+      <c r="D5" s="245" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="338"/>
+      <c r="E5" s="243"/>
       <c r="M5"/>
       <c r="N5"/>
     </row>
@@ -5717,8 +5717,8 @@
       <c r="C6" s="191">
         <v>6</v>
       </c>
-      <c r="D6" s="317"/>
-      <c r="E6" s="338"/>
+      <c r="D6" s="228"/>
+      <c r="E6" s="243"/>
       <c r="M6"/>
       <c r="N6"/>
     </row>
@@ -5733,7 +5733,7 @@
       <c r="D7" s="188" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="338"/>
+      <c r="E7" s="243"/>
       <c r="M7"/>
       <c r="N7"/>
     </row>
@@ -5748,7 +5748,7 @@
       <c r="D8" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="338"/>
+      <c r="E8" s="243"/>
       <c r="M8"/>
       <c r="N8"/>
     </row>
@@ -5763,7 +5763,7 @@
       <c r="D9" s="188" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="338"/>
+      <c r="E9" s="243"/>
       <c r="M9"/>
       <c r="N9"/>
     </row>
@@ -5775,8 +5775,8 @@
       <c r="C10" s="191">
         <v>10</v>
       </c>
-      <c r="D10" s="317"/>
-      <c r="E10" s="338"/>
+      <c r="D10" s="228"/>
+      <c r="E10" s="243"/>
       <c r="M10"/>
       <c r="N10"/>
     </row>
@@ -5791,7 +5791,7 @@
       <c r="D11" s="188">
         <v>97751818</v>
       </c>
-      <c r="E11" s="338"/>
+      <c r="E11" s="243"/>
       <c r="M11"/>
       <c r="N11"/>
     </row>
@@ -5803,10 +5803,10 @@
       <c r="C12" s="191">
         <v>12</v>
       </c>
-      <c r="D12" s="339">
+      <c r="D12" s="244">
         <v>11328816</v>
       </c>
-      <c r="E12" s="338"/>
+      <c r="E12" s="243"/>
       <c r="M12"/>
       <c r="N12"/>
     </row>
@@ -5818,10 +5818,10 @@
       <c r="C13" s="191">
         <v>13</v>
       </c>
-      <c r="D13" s="339">
+      <c r="D13" s="244">
         <v>3203454</v>
       </c>
-      <c r="E13" s="338"/>
+      <c r="E13" s="243"/>
       <c r="M13"/>
       <c r="N13"/>
     </row>
@@ -5834,7 +5834,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="188"/>
-      <c r="E14" s="338"/>
+      <c r="E14" s="243"/>
       <c r="M14"/>
       <c r="N14"/>
     </row>
@@ -5847,7 +5847,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="188"/>
-      <c r="E15" s="338"/>
+      <c r="E15" s="243"/>
       <c r="M15"/>
       <c r="N15"/>
     </row>
@@ -5860,7 +5860,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="63"/>
-      <c r="E16" s="338"/>
+      <c r="E16" s="243"/>
       <c r="M16"/>
       <c r="N16"/>
     </row>
@@ -5873,7 +5873,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="63"/>
-      <c r="E17" s="338"/>
+      <c r="E17" s="243"/>
       <c r="M17"/>
       <c r="N17"/>
     </row>
@@ -5885,8 +5885,8 @@
       <c r="C18" s="191">
         <v>18</v>
       </c>
-      <c r="D18" s="317"/>
-      <c r="E18" s="338"/>
+      <c r="D18" s="228"/>
+      <c r="E18" s="243"/>
       <c r="M18"/>
       <c r="N18"/>
     </row>
@@ -5901,7 +5901,7 @@
       <c r="D19" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="E19" s="338"/>
+      <c r="E19" s="243"/>
       <c r="M19"/>
       <c r="N19"/>
     </row>
@@ -5914,7 +5914,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="63"/>
-      <c r="E20" s="338"/>
+      <c r="E20" s="243"/>
       <c r="M20"/>
       <c r="N20"/>
     </row>
@@ -5927,7 +5927,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="63"/>
-      <c r="E21" s="338"/>
+      <c r="E21" s="243"/>
       <c r="M21"/>
       <c r="N21"/>
     </row>
@@ -5940,7 +5940,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="63"/>
-      <c r="E22" s="338"/>
+      <c r="E22" s="243"/>
       <c r="M22"/>
       <c r="N22"/>
     </row>
@@ -5953,7 +5953,7 @@
         <v>23</v>
       </c>
       <c r="D23" s="63"/>
-      <c r="E23" s="338"/>
+      <c r="E23" s="243"/>
       <c r="M23"/>
       <c r="N23"/>
     </row>
@@ -5968,7 +5968,7 @@
       <c r="D24" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="338"/>
+      <c r="E24" s="243"/>
       <c r="M24"/>
       <c r="N24"/>
     </row>
@@ -5982,10 +5982,10 @@
       <c r="C25" s="199">
         <v>25</v>
       </c>
-      <c r="D25" s="318" t="s">
+      <c r="D25" s="229" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="319"/>
+      <c r="E25" s="230"/>
       <c r="M25"/>
       <c r="N25"/>
     </row>
@@ -5997,10 +5997,10 @@
       <c r="C26" s="199">
         <v>26</v>
       </c>
-      <c r="D26" s="320" t="s">
+      <c r="D26" s="231" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="321"/>
+      <c r="E26" s="232"/>
       <c r="M26"/>
       <c r="N26"/>
     </row>
@@ -6012,10 +6012,10 @@
       <c r="C27" s="199">
         <v>27</v>
       </c>
-      <c r="D27" s="320" t="s">
+      <c r="D27" s="231" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="321" t="s">
+      <c r="E27" s="232" t="s">
         <v>123</v>
       </c>
       <c r="M27"/>
@@ -6029,10 +6029,10 @@
       <c r="C28" s="199">
         <v>28</v>
       </c>
-      <c r="D28" s="322" t="s">
+      <c r="D28" s="233" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="321"/>
+      <c r="E28" s="232"/>
       <c r="M28"/>
       <c r="N28"/>
     </row>
@@ -6044,10 +6044,10 @@
       <c r="C29" s="199">
         <v>29</v>
       </c>
-      <c r="D29" s="323" t="s">
+      <c r="D29" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="321"/>
+      <c r="E29" s="232"/>
       <c r="M29"/>
       <c r="N29"/>
     </row>
@@ -6059,10 +6059,10 @@
       <c r="C30" s="199">
         <v>30</v>
       </c>
-      <c r="D30" s="322" t="s">
+      <c r="D30" s="233" t="s">
         <v>159</v>
       </c>
-      <c r="E30" s="321"/>
+      <c r="E30" s="232"/>
       <c r="M30"/>
       <c r="N30"/>
     </row>
@@ -6074,10 +6074,10 @@
       <c r="C31" s="199">
         <v>31</v>
       </c>
-      <c r="D31" s="323" t="s">
+      <c r="D31" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="321"/>
+      <c r="E31" s="232"/>
       <c r="M31"/>
       <c r="N31"/>
     </row>
@@ -6089,10 +6089,10 @@
       <c r="C32" s="199">
         <v>32</v>
       </c>
-      <c r="D32" s="323" t="s">
+      <c r="D32" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="321"/>
+      <c r="E32" s="232"/>
       <c r="M32"/>
       <c r="N32"/>
     </row>
@@ -6104,10 +6104,10 @@
       <c r="C33" s="199">
         <v>33</v>
       </c>
-      <c r="D33" s="323" t="s">
+      <c r="D33" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="321"/>
+      <c r="E33" s="232"/>
       <c r="M33"/>
       <c r="N33"/>
     </row>
@@ -6119,10 +6119,10 @@
       <c r="C34" s="199">
         <v>34</v>
       </c>
-      <c r="D34" s="323" t="s">
+      <c r="D34" s="234" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="321"/>
+      <c r="E34" s="232"/>
       <c r="M34"/>
       <c r="N34"/>
     </row>
@@ -6134,10 +6134,10 @@
       <c r="C35" s="199">
         <v>35</v>
       </c>
-      <c r="D35" s="323" t="s">
+      <c r="D35" s="234" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="321"/>
+      <c r="E35" s="232"/>
       <c r="M35"/>
       <c r="N35"/>
     </row>
@@ -6149,10 +6149,10 @@
       <c r="C36" s="199">
         <v>36</v>
       </c>
-      <c r="D36" s="323" t="s">
+      <c r="D36" s="234" t="s">
         <v>160</v>
       </c>
-      <c r="E36" s="324"/>
+      <c r="E36" s="235"/>
       <c r="M36"/>
       <c r="N36"/>
     </row>
@@ -6164,15 +6164,15 @@
       <c r="C37" s="199">
         <v>37</v>
       </c>
-      <c r="D37" s="325" t="s">
+      <c r="D37" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="326"/>
+      <c r="E37" s="237"/>
       <c r="M37"/>
       <c r="N37"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="272" t="s">
+      <c r="A38" s="283" t="s">
         <v>131</v>
       </c>
       <c r="B38" s="202" t="s">
@@ -6181,30 +6181,30 @@
       <c r="C38" s="203">
         <v>38</v>
       </c>
-      <c r="D38" s="323" t="s">
+      <c r="D38" s="234" t="s">
         <v>161</v>
       </c>
-      <c r="E38" s="319"/>
+      <c r="E38" s="230"/>
       <c r="M38"/>
       <c r="N38"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A39" s="273"/>
+      <c r="A39" s="284"/>
       <c r="B39" s="204" t="s">
         <v>131</v>
       </c>
       <c r="C39" s="203">
         <v>39</v>
       </c>
-      <c r="D39" s="325" t="s">
+      <c r="D39" s="236" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="326"/>
+      <c r="E39" s="237"/>
       <c r="M39"/>
       <c r="N39"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="274" t="s">
+      <c r="A40" s="285" t="s">
         <v>132</v>
       </c>
       <c r="B40" s="206" t="s">
@@ -6213,30 +6213,30 @@
       <c r="C40" s="207">
         <v>40</v>
       </c>
-      <c r="D40" s="323" t="s">
+      <c r="D40" s="234" t="s">
         <v>161</v>
       </c>
-      <c r="E40" s="319"/>
+      <c r="E40" s="230"/>
       <c r="M40"/>
       <c r="N40"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A41" s="275"/>
+      <c r="A41" s="286"/>
       <c r="B41" s="208" t="s">
         <v>132</v>
       </c>
       <c r="C41" s="207">
         <v>41</v>
       </c>
-      <c r="D41" s="325" t="s">
+      <c r="D41" s="236" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="326"/>
+      <c r="E41" s="237"/>
       <c r="M41"/>
       <c r="N41"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="276" t="s">
+      <c r="A42" s="287" t="s">
         <v>163</v>
       </c>
       <c r="B42" s="209" t="s">
@@ -6245,30 +6245,30 @@
       <c r="C42" s="196">
         <v>42</v>
       </c>
-      <c r="D42" s="323" t="s">
+      <c r="D42" s="234" t="s">
         <v>160</v>
       </c>
-      <c r="E42" s="319"/>
+      <c r="E42" s="230"/>
       <c r="M42"/>
       <c r="N42"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A43" s="277"/>
+      <c r="A43" s="288"/>
       <c r="B43" s="210" t="s">
         <v>165</v>
       </c>
       <c r="C43" s="196">
         <v>43</v>
       </c>
-      <c r="D43" s="325" t="s">
+      <c r="D43" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="326"/>
+      <c r="E43" s="237"/>
       <c r="M43"/>
       <c r="N43"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A44" s="278" t="s">
+      <c r="A44" s="274" t="s">
         <v>150</v>
       </c>
       <c r="B44" s="202" t="s">
@@ -6277,30 +6277,30 @@
       <c r="C44" s="203">
         <v>44</v>
       </c>
-      <c r="D44" s="325" t="s">
+      <c r="D44" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="319"/>
+      <c r="E44" s="230"/>
       <c r="M44"/>
       <c r="N44"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A45" s="279"/>
+      <c r="A45" s="276"/>
       <c r="B45" s="204" t="s">
         <v>147</v>
       </c>
       <c r="C45" s="203">
         <v>45</v>
       </c>
-      <c r="D45" s="325" t="s">
+      <c r="D45" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="326"/>
+      <c r="E45" s="237"/>
       <c r="M45"/>
       <c r="N45"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="280" t="s">
+      <c r="A46" s="289" t="s">
         <v>151</v>
       </c>
       <c r="B46" s="198" t="s">
@@ -6309,45 +6309,45 @@
       <c r="C46" s="199">
         <v>46</v>
       </c>
-      <c r="D46" s="322" t="s">
+      <c r="D46" s="233" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="319"/>
+      <c r="E46" s="230"/>
       <c r="M46"/>
       <c r="N46"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="281"/>
+      <c r="A47" s="290"/>
       <c r="B47" s="200" t="s">
         <v>117</v>
       </c>
       <c r="C47" s="199">
         <v>47</v>
       </c>
-      <c r="D47" s="327" t="s">
+      <c r="D47" s="277" t="s">
         <v>118</v>
       </c>
-      <c r="E47" s="328"/>
+      <c r="E47" s="278"/>
       <c r="M47"/>
       <c r="N47"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A48" s="282"/>
+      <c r="A48" s="291"/>
       <c r="B48" s="201" t="s">
         <v>119</v>
       </c>
       <c r="C48" s="199">
         <v>48</v>
       </c>
-      <c r="D48" s="329" t="s">
+      <c r="D48" s="279" t="s">
         <v>118</v>
       </c>
-      <c r="E48" s="330"/>
+      <c r="E48" s="280"/>
       <c r="M48"/>
       <c r="N48"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="278" t="s">
+      <c r="A49" s="274" t="s">
         <v>152</v>
       </c>
       <c r="B49" s="202" t="s">
@@ -6356,45 +6356,45 @@
       <c r="C49" s="203">
         <v>49</v>
       </c>
-      <c r="D49" s="322" t="s">
+      <c r="D49" s="233" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="331"/>
+      <c r="E49" s="238"/>
       <c r="M49"/>
       <c r="N49"/>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="283"/>
+      <c r="A50" s="275"/>
       <c r="B50" s="211" t="s">
         <v>128</v>
       </c>
       <c r="C50" s="203">
         <v>50</v>
       </c>
-      <c r="D50" s="323" t="s">
+      <c r="D50" s="234" t="s">
         <v>155</v>
       </c>
-      <c r="E50" s="332"/>
+      <c r="E50" s="239"/>
       <c r="M50"/>
       <c r="N50"/>
     </row>
     <row r="51" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A51" s="279"/>
+      <c r="A51" s="276"/>
       <c r="B51" s="204" t="s">
         <v>134</v>
       </c>
       <c r="C51" s="203">
         <v>51</v>
       </c>
-      <c r="D51" s="325" t="s">
+      <c r="D51" s="236" t="s">
         <v>155</v>
       </c>
-      <c r="E51" s="333"/>
+      <c r="E51" s="240"/>
       <c r="M51"/>
       <c r="N51"/>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="266" t="s">
+      <c r="A52" s="302" t="s">
         <v>153</v>
       </c>
       <c r="B52" s="206" t="s">
@@ -6403,60 +6403,60 @@
       <c r="C52" s="207">
         <v>52</v>
       </c>
-      <c r="D52" s="322" t="s">
+      <c r="D52" s="233" t="s">
         <v>71</v>
       </c>
-      <c r="E52" s="331"/>
+      <c r="E52" s="238"/>
       <c r="M52"/>
       <c r="N52"/>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="267"/>
+      <c r="A53" s="303"/>
       <c r="B53" s="212" t="s">
         <v>145</v>
       </c>
       <c r="C53" s="207">
         <v>53</v>
       </c>
-      <c r="D53" s="323" t="s">
+      <c r="D53" s="234" t="s">
         <v>146</v>
       </c>
-      <c r="E53" s="332"/>
+      <c r="E53" s="239"/>
       <c r="M53"/>
       <c r="N53"/>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="267"/>
+      <c r="A54" s="303"/>
       <c r="B54" s="212" t="s">
         <v>142</v>
       </c>
       <c r="C54" s="207">
         <v>54</v>
       </c>
-      <c r="D54" s="323" t="s">
+      <c r="D54" s="234" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="332"/>
+      <c r="E54" s="239"/>
       <c r="M54"/>
       <c r="N54"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A55" s="268"/>
+      <c r="A55" s="304"/>
       <c r="B55" s="208" t="s">
         <v>144</v>
       </c>
       <c r="C55" s="207">
         <v>55</v>
       </c>
-      <c r="D55" s="325" t="s">
+      <c r="D55" s="236" t="s">
         <v>146</v>
       </c>
-      <c r="E55" s="333"/>
+      <c r="E55" s="240"/>
       <c r="M55"/>
       <c r="N55"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="269" t="s">
+      <c r="A56" s="305" t="s">
         <v>157</v>
       </c>
       <c r="B56" s="213" t="s">
@@ -6465,45 +6465,45 @@
       <c r="C56" s="196">
         <v>56</v>
       </c>
-      <c r="D56" s="334" t="s">
+      <c r="D56" s="281" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="335"/>
+      <c r="E56" s="282"/>
       <c r="M56"/>
       <c r="N56"/>
     </row>
     <row r="57" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A57" s="270"/>
+      <c r="A57" s="306"/>
       <c r="B57" s="214" t="s">
         <v>167</v>
       </c>
       <c r="C57" s="196">
         <v>57</v>
       </c>
-      <c r="D57" s="325" t="s">
+      <c r="D57" s="236" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="336"/>
+      <c r="E57" s="241"/>
       <c r="M57"/>
       <c r="N57"/>
     </row>
     <row r="58" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A58" s="271"/>
+      <c r="A58" s="307"/>
       <c r="B58" s="215" t="s">
         <v>156</v>
       </c>
       <c r="C58" s="196">
         <v>58</v>
       </c>
-      <c r="D58" s="325" t="s">
+      <c r="D58" s="236" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="326"/>
+      <c r="E58" s="237"/>
       <c r="M58"/>
       <c r="N58"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="256" t="s">
+      <c r="A59" s="292" t="s">
         <v>85</v>
       </c>
       <c r="B59" s="216" t="s">
@@ -6516,7 +6516,7 @@
       <c r="N59"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="257"/>
+      <c r="A60" s="293"/>
       <c r="B60" s="203" t="s">
         <v>389</v>
       </c>
@@ -6527,7 +6527,7 @@
       <c r="N60"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="257"/>
+      <c r="A61" s="293"/>
       <c r="B61" s="216" t="s">
         <v>390</v>
       </c>
@@ -6536,7 +6536,7 @@
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="257"/>
+      <c r="A62" s="293"/>
       <c r="B62" s="217" t="s">
         <v>64</v>
       </c>
@@ -6545,7 +6545,7 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="258"/>
+      <c r="A63" s="294"/>
       <c r="B63" s="218" t="s">
         <v>204</v>
       </c>
@@ -6554,7 +6554,7 @@
       </c>
     </row>
     <row r="64" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A64" s="259"/>
+      <c r="A64" s="295"/>
       <c r="B64" s="219" t="s">
         <v>68</v>
       </c>
@@ -6725,7 +6725,7 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="260" t="s">
+      <c r="A83" s="296" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="213" t="s">
@@ -6736,7 +6736,7 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="261"/>
+      <c r="A84" s="297"/>
       <c r="B84" s="222" t="s">
         <v>390</v>
       </c>
@@ -6745,7 +6745,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="261"/>
+      <c r="A85" s="297"/>
       <c r="B85" s="222" t="s">
         <v>115</v>
       </c>
@@ -6754,7 +6754,7 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="261"/>
+      <c r="A86" s="297"/>
       <c r="B86" s="222" t="s">
         <v>86</v>
       </c>
@@ -6763,7 +6763,7 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="261"/>
+      <c r="A87" s="297"/>
       <c r="B87" s="223" t="s">
         <v>64</v>
       </c>
@@ -6772,7 +6772,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A88" s="262"/>
+      <c r="A88" s="298"/>
       <c r="B88" s="224" t="s">
         <v>68</v>
       </c>
@@ -6943,7 +6943,7 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="263" t="s">
+      <c r="A107" s="299" t="s">
         <v>84</v>
       </c>
       <c r="B107" s="119" t="s">
@@ -6954,7 +6954,7 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="264"/>
+      <c r="A108" s="300"/>
       <c r="B108" s="119" t="s">
         <v>109</v>
       </c>
@@ -6963,7 +6963,7 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="264"/>
+      <c r="A109" s="300"/>
       <c r="B109" s="119" t="s">
         <v>389</v>
       </c>
@@ -6972,7 +6972,7 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="264"/>
+      <c r="A110" s="300"/>
       <c r="B110" s="225" t="s">
         <v>390</v>
       </c>
@@ -6981,7 +6981,7 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="264"/>
+      <c r="A111" s="300"/>
       <c r="B111" s="119" t="s">
         <v>113</v>
       </c>
@@ -6990,7 +6990,7 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="264"/>
+      <c r="A112" s="300"/>
       <c r="B112" s="119" t="s">
         <v>86</v>
       </c>
@@ -6999,7 +6999,7 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="264"/>
+      <c r="A113" s="300"/>
       <c r="B113" s="226" t="s">
         <v>64</v>
       </c>
@@ -7008,7 +7008,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A114" s="265"/>
+      <c r="A114" s="301"/>
       <c r="B114" s="227" t="s">
         <v>68</v>
       </c>
@@ -7234,6 +7234,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A83:A88"/>
+    <mergeCell ref="A107:A114"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A58"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
@@ -7243,11 +7248,6 @@
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A83:A88"/>
-    <mergeCell ref="A107:A114"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A56:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -7258,8 +7258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7272,15 +7272,15 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B2" s="286" t="s">
+      <c r="B2" s="310" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="288"/>
+      <c r="C2" s="311"/>
+      <c r="D2" s="311"/>
+      <c r="E2" s="312"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="289" t="s">
+      <c r="B3" s="313" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="118" t="s">
@@ -7294,7 +7294,7 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="290"/>
+      <c r="B4" s="314"/>
       <c r="C4" s="64" t="s">
         <v>193</v>
       </c>
@@ -7304,7 +7304,7 @@
       <c r="E4" s="67"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="290"/>
+      <c r="B5" s="314"/>
       <c r="C5" s="64" t="s">
         <v>195</v>
       </c>
@@ -7314,7 +7314,7 @@
       <c r="E5" s="67"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="290"/>
+      <c r="B6" s="314"/>
       <c r="C6" s="64" t="s">
         <v>197</v>
       </c>
@@ -7324,7 +7324,7 @@
       <c r="E6" s="67"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="290"/>
+      <c r="B7" s="314"/>
       <c r="C7" s="64" t="s">
         <v>198</v>
       </c>
@@ -7334,7 +7334,7 @@
       <c r="E7" s="67"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="290"/>
+      <c r="B8" s="314"/>
       <c r="C8" s="64" t="s">
         <v>205</v>
       </c>
@@ -7342,7 +7342,7 @@
       <c r="E8" s="67"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="290"/>
+      <c r="B9" s="314"/>
       <c r="C9" s="64" t="s">
         <v>206</v>
       </c>
@@ -7350,7 +7350,7 @@
       <c r="E9" s="67"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="290"/>
+      <c r="B10" s="314"/>
       <c r="C10" s="64" t="s">
         <v>200</v>
       </c>
@@ -7358,7 +7358,7 @@
       <c r="E10" s="88"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="290"/>
+      <c r="B11" s="314"/>
       <c r="C11" s="64" t="s">
         <v>72</v>
       </c>
@@ -7368,7 +7368,7 @@
       <c r="E11" s="88"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="290"/>
+      <c r="B12" s="314"/>
       <c r="C12" s="119" t="s">
         <v>214</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="E12" s="89"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="290"/>
+      <c r="B13" s="314"/>
       <c r="C13" s="119" t="s">
         <v>216</v>
       </c>
@@ -7386,7 +7386,7 @@
       <c r="E13" s="89"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="290"/>
+      <c r="B14" s="314"/>
       <c r="C14" s="119" t="s">
         <v>217</v>
       </c>
@@ -7394,7 +7394,7 @@
       <c r="E14" s="89"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="290"/>
+      <c r="B15" s="314"/>
       <c r="C15" s="119" t="s">
         <v>218</v>
       </c>
@@ -7404,7 +7404,7 @@
       <c r="E15" s="89"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="290"/>
+      <c r="B16" s="314"/>
       <c r="C16" s="119" t="s">
         <v>219</v>
       </c>
@@ -7412,7 +7412,7 @@
       <c r="E16" s="89"/>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="290"/>
+      <c r="B17" s="314"/>
       <c r="C17" s="119" t="s">
         <v>220</v>
       </c>
@@ -7420,7 +7420,7 @@
       <c r="E17" s="65"/>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="290"/>
+      <c r="B18" s="314"/>
       <c r="C18" s="119" t="s">
         <v>221</v>
       </c>
@@ -7430,7 +7430,7 @@
       <c r="E18" s="65"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="290"/>
+      <c r="B19" s="314"/>
       <c r="C19" s="120" t="s">
         <v>210</v>
       </c>
@@ -7440,7 +7440,7 @@
       <c r="E19" s="65"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="290"/>
+      <c r="B20" s="314"/>
       <c r="C20" s="120" t="s">
         <v>208</v>
       </c>
@@ -7452,7 +7452,7 @@
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="290"/>
+      <c r="B21" s="314"/>
       <c r="C21" s="120" t="s">
         <v>211</v>
       </c>
@@ -7462,7 +7462,7 @@
       <c r="E21" s="65"/>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="290"/>
+      <c r="B22" s="314"/>
       <c r="C22" s="120" t="s">
         <v>208</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="E22" s="65"/>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="290"/>
+      <c r="B23" s="314"/>
       <c r="C23" s="120" t="s">
         <v>212</v>
       </c>
@@ -7482,7 +7482,7 @@
       <c r="E23" s="67"/>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="290"/>
+      <c r="B24" s="314"/>
       <c r="C24" s="120" t="s">
         <v>208</v>
       </c>
@@ -7492,7 +7492,7 @@
       <c r="E24" s="67"/>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="290"/>
+      <c r="B25" s="314"/>
       <c r="C25" s="120" t="s">
         <v>213</v>
       </c>
@@ -7502,7 +7502,7 @@
       <c r="E25" s="67"/>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="290"/>
+      <c r="B26" s="314"/>
       <c r="C26" s="120" t="s">
         <v>208</v>
       </c>
@@ -7512,7 +7512,7 @@
       <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B27" s="290"/>
+      <c r="B27" s="314"/>
       <c r="C27" s="121" t="s">
         <v>222</v>
       </c>
@@ -7522,7 +7522,7 @@
       <c r="E27" s="102"/>
     </row>
     <row r="28" spans="2:5" ht="14.45" customHeight="1">
-      <c r="B28" s="291" t="s">
+      <c r="B28" s="315" t="s">
         <v>148</v>
       </c>
       <c r="C28" s="126" t="s">
@@ -7534,7 +7534,7 @@
       <c r="E28" s="87"/>
     </row>
     <row r="29" spans="2:5" ht="14.45" customHeight="1">
-      <c r="B29" s="292"/>
+      <c r="B29" s="316"/>
       <c r="C29" s="78" t="s">
         <v>126</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="E29" s="67"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="292"/>
+      <c r="B30" s="316"/>
       <c r="C30" s="78" t="s">
         <v>124</v>
       </c>
@@ -7554,7 +7554,7 @@
       <c r="E30" s="67"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="292"/>
+      <c r="B31" s="316"/>
       <c r="C31" s="78" t="s">
         <v>129</v>
       </c>
@@ -7564,7 +7564,7 @@
       <c r="E31" s="122"/>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="292"/>
+      <c r="B32" s="316"/>
       <c r="C32" s="78" t="s">
         <v>138</v>
       </c>
@@ -7574,7 +7574,7 @@
       <c r="E32" s="122"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B33" s="293"/>
+      <c r="B33" s="317"/>
       <c r="C33" s="127" t="s">
         <v>130</v>
       </c>
@@ -7584,7 +7584,7 @@
       <c r="E33" s="129"/>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="289" t="s">
+      <c r="B34" s="313" t="s">
         <v>227</v>
       </c>
       <c r="C34" s="133" t="s">
@@ -7596,7 +7596,7 @@
       <c r="E34" s="130"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="290"/>
+      <c r="B35" s="314"/>
       <c r="C35" s="134" t="s">
         <v>224</v>
       </c>
@@ -7606,7 +7606,7 @@
       <c r="E35" s="67"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="290"/>
+      <c r="B36" s="314"/>
       <c r="C36" s="134" t="s">
         <v>228</v>
       </c>
@@ -7616,7 +7616,7 @@
       <c r="E36" s="67"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B37" s="294"/>
+      <c r="B37" s="318"/>
       <c r="C37" s="135" t="s">
         <v>226</v>
       </c>
@@ -7626,7 +7626,7 @@
       <c r="E37" s="92"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="240" t="s">
+      <c r="B38" s="261" t="s">
         <v>229</v>
       </c>
       <c r="C38" s="113" t="s">
@@ -7638,27 +7638,27 @@
       <c r="E38" s="87"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="241"/>
+      <c r="B39" s="273"/>
       <c r="C39" s="136" t="s">
         <v>233</v>
       </c>
-      <c r="D39" s="250" t="s">
+      <c r="D39" s="248" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="251"/>
+      <c r="E39" s="249"/>
     </row>
     <row r="40" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B40" s="241"/>
+      <c r="B40" s="273"/>
       <c r="C40" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="D40" s="284" t="s">
+      <c r="D40" s="308" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="285"/>
+      <c r="E40" s="309"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="243" t="s">
+      <c r="B41" s="254" t="s">
         <v>157</v>
       </c>
       <c r="C41" s="93" t="s">
@@ -7670,7 +7670,7 @@
       <c r="E41" s="98"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B42" s="245"/>
+      <c r="B42" s="256"/>
       <c r="C42" s="95" t="s">
         <v>156</v>
       </c>
@@ -7713,15 +7713,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.15" customHeight="1" thickBot="1">
-      <c r="B1" s="296" t="s">
+      <c r="B1" s="320" t="s">
         <v>367</v>
       </c>
-      <c r="C1" s="296"/>
-      <c r="D1" s="296"/>
-      <c r="E1" s="296"/>
+      <c r="C1" s="320"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
     </row>
     <row r="2" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="266" t="s">
         <v>189</v>
       </c>
       <c r="C2" s="111" t="s">
@@ -7733,7 +7733,7 @@
       <c r="E2" s="87"/>
     </row>
     <row r="3" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B3" s="234"/>
+      <c r="B3" s="267"/>
       <c r="C3" s="109" t="s">
         <v>168</v>
       </c>
@@ -7743,7 +7743,7 @@
       <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B4" s="234"/>
+      <c r="B4" s="267"/>
       <c r="C4" s="109" t="s">
         <v>327</v>
       </c>
@@ -7753,7 +7753,7 @@
       <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B5" s="234"/>
+      <c r="B5" s="267"/>
       <c r="C5" s="109" t="s">
         <v>170</v>
       </c>
@@ -7765,7 +7765,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.15" customHeight="1">
-      <c r="B6" s="234"/>
+      <c r="B6" s="267"/>
       <c r="C6" s="109" t="s">
         <v>174</v>
       </c>
@@ -7777,7 +7777,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B7" s="234"/>
+      <c r="B7" s="267"/>
       <c r="C7" s="109" t="s">
         <v>171</v>
       </c>
@@ -7789,7 +7789,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B8" s="234"/>
+      <c r="B8" s="267"/>
       <c r="C8" s="109" t="s">
         <v>172</v>
       </c>
@@ -7801,7 +7801,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B9" s="234"/>
+      <c r="B9" s="267"/>
       <c r="C9" s="109" t="s">
         <v>177</v>
       </c>
@@ -7813,7 +7813,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B10" s="234"/>
+      <c r="B10" s="267"/>
       <c r="C10" s="109" t="s">
         <v>173</v>
       </c>
@@ -7823,7 +7823,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.45" customHeight="1">
-      <c r="B11" s="234"/>
+      <c r="B11" s="267"/>
       <c r="C11" s="109" t="s">
         <v>182</v>
       </c>
@@ -7835,7 +7835,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17.45" customHeight="1" thickBot="1">
-      <c r="B12" s="235"/>
+      <c r="B12" s="268"/>
       <c r="C12" s="112" t="s">
         <v>180</v>
       </c>
@@ -7847,11 +7847,11 @@
     <row r="13" spans="1:5" ht="17.45" customHeight="1"/>
     <row r="14" spans="1:5" ht="17.45" customHeight="1"/>
     <row r="15" spans="1:5" ht="40.15" customHeight="1">
-      <c r="A15" s="295" t="s">
+      <c r="A15" s="319" t="s">
         <v>326</v>
       </c>
-      <c r="B15" s="295"/>
-      <c r="C15" s="295"/>
+      <c r="B15" s="319"/>
+      <c r="C15" s="319"/>
     </row>
     <row r="16" spans="1:5" ht="40.15" customHeight="1">
       <c r="A16" s="139" t="s">
@@ -8065,7 +8065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -8076,18 +8076,18 @@
   <sheetData>
     <row r="1" spans="1:15" ht="52.9" customHeight="1" thickBot="1">
       <c r="A1" s="176"/>
-      <c r="B1" s="297" t="s">
+      <c r="B1" s="321" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="298"/>
-      <c r="D1" s="298"/>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
-      <c r="J1" s="298"/>
-      <c r="K1" s="298"/>
+      <c r="C1" s="322"/>
+      <c r="D1" s="322"/>
+      <c r="E1" s="322"/>
+      <c r="F1" s="322"/>
+      <c r="G1" s="322"/>
+      <c r="H1" s="322"/>
+      <c r="I1" s="322"/>
+      <c r="J1" s="322"/>
+      <c r="K1" s="322"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -8193,7 +8193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="C35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
@@ -8208,13 +8208,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25">
-      <c r="A1" s="304" t="s">
+      <c r="A1" s="328" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="304"/>
-      <c r="C1" s="304"/>
-      <c r="D1" s="304"/>
-      <c r="E1" s="304"/>
+      <c r="B1" s="328"/>
+      <c r="C1" s="328"/>
+      <c r="D1" s="328"/>
+      <c r="E1" s="328"/>
     </row>
     <row r="2" spans="1:12" ht="24" thickBot="1">
       <c r="A2" s="145"/>
@@ -8226,17 +8226,17 @@
         <v>240</v>
       </c>
       <c r="E2" s="145"/>
-      <c r="G2" s="301" t="s">
+      <c r="G2" s="325" t="s">
         <v>328</v>
       </c>
-      <c r="H2" s="301"/>
+      <c r="H2" s="325"/>
       <c r="I2" s="175" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
       <c r="A3" s="148"/>
-      <c r="B3" s="305" t="s">
+      <c r="B3" s="329" t="s">
         <v>286</v>
       </c>
       <c r="C3" s="154">
@@ -8255,7 +8255,7 @@
     </row>
     <row r="4" spans="1:12" ht="35.450000000000003" customHeight="1" thickBot="1">
       <c r="A4" s="148"/>
-      <c r="B4" s="305"/>
+      <c r="B4" s="329"/>
       <c r="C4" s="154">
         <v>103</v>
       </c>
@@ -8269,7 +8269,7 @@
       <c r="H4" s="160" t="s">
         <v>339</v>
       </c>
-      <c r="I4" s="302" t="s">
+      <c r="I4" s="326" t="s">
         <v>331</v>
       </c>
       <c r="K4" s="152"/>
@@ -8277,7 +8277,7 @@
     </row>
     <row r="5" spans="1:12" ht="94.5" thickBot="1">
       <c r="A5" s="148"/>
-      <c r="B5" s="305"/>
+      <c r="B5" s="329"/>
       <c r="C5" s="154">
         <v>105</v>
       </c>
@@ -8289,11 +8289,11 @@
       <c r="H5" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="303"/>
+      <c r="I5" s="327"/>
     </row>
     <row r="6" spans="1:12" ht="19.5" thickBot="1">
       <c r="A6" s="148"/>
-      <c r="B6" s="305"/>
+      <c r="B6" s="329"/>
       <c r="C6" s="154">
         <v>107</v>
       </c>
@@ -8313,7 +8313,7 @@
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
       <c r="A7" s="148"/>
-      <c r="B7" s="305"/>
+      <c r="B7" s="329"/>
       <c r="C7" s="154">
         <v>109</v>
       </c>
@@ -8333,7 +8333,7 @@
     </row>
     <row r="8" spans="1:12" ht="75.75" thickBot="1">
       <c r="A8" s="148"/>
-      <c r="B8" s="305"/>
+      <c r="B8" s="329"/>
       <c r="C8" s="154">
         <v>111</v>
       </c>
@@ -8353,7 +8353,7 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="148"/>
-      <c r="B9" s="305"/>
+      <c r="B9" s="329"/>
       <c r="C9" s="154">
         <v>113</v>
       </c>
@@ -8364,7 +8364,7 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1">
       <c r="A10" s="148"/>
-      <c r="B10" s="305"/>
+      <c r="B10" s="329"/>
       <c r="C10" s="154">
         <v>115</v>
       </c>
@@ -8375,7 +8375,7 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1">
       <c r="A11" s="148"/>
-      <c r="B11" s="305"/>
+      <c r="B11" s="329"/>
       <c r="C11" s="154">
         <v>117</v>
       </c>
@@ -8386,7 +8386,7 @@
     </row>
     <row r="12" spans="1:12" ht="70.900000000000006" customHeight="1" thickBot="1">
       <c r="A12" s="148"/>
-      <c r="B12" s="305"/>
+      <c r="B12" s="329"/>
       <c r="C12" s="154">
         <v>119</v>
       </c>
@@ -8397,7 +8397,7 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" s="148"/>
-      <c r="B13" s="306" t="s">
+      <c r="B13" s="330" t="s">
         <v>296</v>
       </c>
       <c r="C13" s="154">
@@ -8410,7 +8410,7 @@
     </row>
     <row r="14" spans="1:12" ht="24.75" thickBot="1">
       <c r="A14" s="148"/>
-      <c r="B14" s="299"/>
+      <c r="B14" s="323"/>
       <c r="C14" s="154">
         <v>203</v>
       </c>
@@ -8421,7 +8421,7 @@
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="148"/>
-      <c r="B15" s="299"/>
+      <c r="B15" s="323"/>
       <c r="C15" s="154">
         <v>205</v>
       </c>
@@ -8432,7 +8432,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="148"/>
-      <c r="B16" s="300"/>
+      <c r="B16" s="324"/>
       <c r="C16" s="154">
         <v>207</v>
       </c>
@@ -8443,7 +8443,7 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="148"/>
-      <c r="B17" s="306" t="s">
+      <c r="B17" s="330" t="s">
         <v>301</v>
       </c>
       <c r="C17" s="154">
@@ -8456,7 +8456,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="148"/>
-      <c r="B18" s="299"/>
+      <c r="B18" s="323"/>
       <c r="C18" s="154">
         <v>303</v>
       </c>
@@ -8467,7 +8467,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="148"/>
-      <c r="B19" s="299"/>
+      <c r="B19" s="323"/>
       <c r="C19" s="154">
         <v>305</v>
       </c>
@@ -8478,7 +8478,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="148"/>
-      <c r="B20" s="299"/>
+      <c r="B20" s="323"/>
       <c r="C20" s="154">
         <v>307</v>
       </c>
@@ -8489,7 +8489,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1">
       <c r="A21" s="148"/>
-      <c r="B21" s="299"/>
+      <c r="B21" s="323"/>
       <c r="C21" s="154">
         <v>309</v>
       </c>
@@ -8500,7 +8500,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1">
       <c r="A22" s="148"/>
-      <c r="B22" s="299"/>
+      <c r="B22" s="323"/>
       <c r="C22" s="154">
         <v>311</v>
       </c>
@@ -8511,7 +8511,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
       <c r="A23" s="148"/>
-      <c r="B23" s="299"/>
+      <c r="B23" s="323"/>
       <c r="C23" s="154">
         <v>313</v>
       </c>
@@ -8522,7 +8522,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="148"/>
-      <c r="B24" s="299"/>
+      <c r="B24" s="323"/>
       <c r="C24" s="154">
         <v>315</v>
       </c>
@@ -8533,7 +8533,7 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1">
       <c r="A25" s="148"/>
-      <c r="B25" s="307" t="s">
+      <c r="B25" s="331" t="s">
         <v>308</v>
       </c>
       <c r="C25" s="154">
@@ -8546,7 +8546,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1">
       <c r="A26" s="148"/>
-      <c r="B26" s="308"/>
+      <c r="B26" s="332"/>
       <c r="C26" s="154">
         <v>403</v>
       </c>
@@ -8557,7 +8557,7 @@
     </row>
     <row r="27" spans="1:5" ht="24.75" thickBot="1">
       <c r="A27" s="148"/>
-      <c r="B27" s="308"/>
+      <c r="B27" s="332"/>
       <c r="C27" s="154">
         <v>405</v>
       </c>
@@ -8568,7 +8568,7 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1">
       <c r="A28" s="148"/>
-      <c r="B28" s="308"/>
+      <c r="B28" s="332"/>
       <c r="C28" s="154">
         <v>407</v>
       </c>
@@ -8579,7 +8579,7 @@
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="148"/>
-      <c r="B29" s="308"/>
+      <c r="B29" s="332"/>
       <c r="C29" s="154">
         <v>409</v>
       </c>
@@ -8590,7 +8590,7 @@
     </row>
     <row r="30" spans="1:5" ht="24.75" thickBot="1">
       <c r="A30" s="148"/>
-      <c r="B30" s="308"/>
+      <c r="B30" s="332"/>
       <c r="C30" s="154">
         <v>411</v>
       </c>
@@ -8601,7 +8601,7 @@
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1">
       <c r="A31" s="148"/>
-      <c r="B31" s="308"/>
+      <c r="B31" s="332"/>
       <c r="C31" s="154">
         <v>413</v>
       </c>
@@ -8612,7 +8612,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1">
       <c r="A32" s="148"/>
-      <c r="B32" s="308"/>
+      <c r="B32" s="332"/>
       <c r="C32" s="154">
         <v>415</v>
       </c>
@@ -8623,7 +8623,7 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1">
       <c r="A33" s="148"/>
-      <c r="B33" s="308"/>
+      <c r="B33" s="332"/>
       <c r="C33" s="154">
         <v>417</v>
       </c>
@@ -8634,7 +8634,7 @@
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1">
       <c r="A34" s="148"/>
-      <c r="B34" s="309"/>
+      <c r="B34" s="333"/>
       <c r="C34" s="154">
         <v>419</v>
       </c>
@@ -8644,7 +8644,7 @@
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1">
       <c r="A35" s="148"/>
-      <c r="B35" s="299" t="s">
+      <c r="B35" s="323" t="s">
         <v>319</v>
       </c>
       <c r="C35" s="154">
@@ -8656,7 +8656,7 @@
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1">
       <c r="A36" s="148"/>
-      <c r="B36" s="299"/>
+      <c r="B36" s="323"/>
       <c r="C36" s="154">
         <v>503</v>
       </c>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="37" spans="1:5" ht="24.75" thickBot="1">
       <c r="A37" s="148"/>
-      <c r="B37" s="299"/>
+      <c r="B37" s="323"/>
       <c r="C37" s="154">
         <v>505</v>
       </c>
@@ -8678,7 +8678,7 @@
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1">
       <c r="A38" s="148"/>
-      <c r="B38" s="299"/>
+      <c r="B38" s="323"/>
       <c r="C38" s="154">
         <v>507</v>
       </c>
@@ -8688,7 +8688,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" thickBot="1">
       <c r="A39" s="148"/>
-      <c r="B39" s="299"/>
+      <c r="B39" s="323"/>
       <c r="C39" s="154">
         <v>509</v>
       </c>
@@ -8699,7 +8699,7 @@
     </row>
     <row r="40" spans="1:5" ht="36.75" thickBot="1">
       <c r="A40" s="148"/>
-      <c r="B40" s="299"/>
+      <c r="B40" s="323"/>
       <c r="C40" s="154">
         <v>511</v>
       </c>
@@ -8710,7 +8710,7 @@
     </row>
     <row r="41" spans="1:5" ht="24.75" thickBot="1">
       <c r="A41" s="148"/>
-      <c r="B41" s="300"/>
+      <c r="B41" s="324"/>
       <c r="C41" s="154">
         <v>513</v>
       </c>
@@ -8759,47 +8759,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="67.150000000000006" customHeight="1">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="337" t="s">
         <v>368</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
-      <c r="E1" s="313"/>
+      <c r="B1" s="337"/>
+      <c r="C1" s="337"/>
+      <c r="D1" s="337"/>
+      <c r="E1" s="337"/>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="314" t="s">
+      <c r="A2" s="338" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="314"/>
-      <c r="C2" s="314"/>
-      <c r="D2" s="314"/>
-      <c r="E2" s="314"/>
-      <c r="F2" s="314"/>
+      <c r="B2" s="338"/>
+      <c r="C2" s="338"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338"/>
+      <c r="F2" s="338"/>
     </row>
     <row r="3" spans="1:6" ht="28.5">
       <c r="A3" s="171" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="310" t="s">
+      <c r="B3" s="334" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="310"/>
-      <c r="D3" s="310"/>
-      <c r="E3" s="310"/>
-      <c r="F3" s="310"/>
+      <c r="C3" s="334"/>
+      <c r="D3" s="334"/>
+      <c r="E3" s="334"/>
+      <c r="F3" s="334"/>
     </row>
     <row r="4" spans="1:6" ht="30">
       <c r="A4" s="170" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="311" t="s">
+      <c r="B4" s="335" t="s">
         <v>359</v>
       </c>
-      <c r="C4" s="311"/>
-      <c r="D4" s="311"/>
-      <c r="E4" s="311"/>
-      <c r="F4" s="311"/>
+      <c r="C4" s="335"/>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="335"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="166" t="s">
@@ -8889,13 +8889,13 @@
       <c r="A10" s="170" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="312" t="s">
+      <c r="B10" s="336" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="312"/>
-      <c r="D10" s="312"/>
-      <c r="E10" s="312"/>
-      <c r="F10" s="312"/>
+      <c r="C10" s="336"/>
+      <c r="D10" s="336"/>
+      <c r="E10" s="336"/>
+      <c r="F10" s="336"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="166" t="s">
@@ -9021,24 +9021,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="42" customHeight="1">
-      <c r="A1" s="315" t="s">
+      <c r="A1" s="339" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="315"/>
-      <c r="C1" s="315"/>
-      <c r="D1" s="315"/>
-      <c r="E1" s="315"/>
-      <c r="F1" s="315"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="339"/>
     </row>
     <row r="2" spans="1:8" ht="42" customHeight="1">
-      <c r="A2" s="316" t="s">
+      <c r="A2" s="340" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="316"/>
-      <c r="C2" s="316"/>
-      <c r="D2" s="316"/>
-      <c r="E2" s="316"/>
-      <c r="F2" s="316"/>
+      <c r="B2" s="340"/>
+      <c r="C2" s="340"/>
+      <c r="D2" s="340"/>
+      <c r="E2" s="340"/>
+      <c r="F2" s="340"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="169" t="s">

</xml_diff>